<commit_message>
added skeleton for the reading of the excel file prices
</commit_message>
<xml_diff>
--- a/prices.xlsx
+++ b/prices.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\TEKLACKE 2018\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="e:\Users\Ramon\Desktop\cursojs\AdminR\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="800" yWindow="1860" windowWidth="19670" windowHeight="5210"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12300"/>
   </bookViews>
   <sheets>
     <sheet name="PINTURAS PARA SUELOS   ABRIL18" sheetId="5" r:id="rId1"/>
@@ -18,12 +18,12 @@
     <sheet name="ACRILICAS ALTA CALIDAD-  (2)" sheetId="7" r:id="rId4"/>
     <sheet name="ENEKRIL FALLAS" sheetId="4" r:id="rId5"/>
   </sheets>
-  <calcPr calcId="152511"/>
+  <calcPr calcId="162913"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="602" uniqueCount="315">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="603" uniqueCount="316">
   <si>
     <t>Nº</t>
   </si>
@@ -981,11 +981,14 @@
   <si>
     <t>ENEKRIL SUELOS 1023/1026</t>
   </si>
+  <si>
+    <t>PASTAS PIGMENTARIAS</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="31" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -2930,7 +2933,7 @@
         <xdr:cNvPr id="4099" name="4 Imagen" descr="teclacke.png">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-000003100000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000003100000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2987,7 +2990,7 @@
         <xdr:cNvPr id="2" name="4 Imagen" descr="teclacke.png">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0100-000002000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-000002000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -3044,7 +3047,7 @@
         <xdr:cNvPr id="3075" name="4 Imagen" descr="teclacke.png">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0200-0000030C0000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0200-0000030C0000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -3101,7 +3104,7 @@
         <xdr:cNvPr id="2" name="4 Imagen" descr="teclacke.png">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0300-000002000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0300-000002000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -3158,7 +3161,7 @@
         <xdr:cNvPr id="2051" name="4 Imagen" descr="teclacke.png">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0400-000003080000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0400-000003080000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -3196,7 +3199,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Tema de Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -3484,75 +3487,75 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:BQ164"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A61" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="AX124" sqref="AX124"/>
+    <sheetView tabSelected="1" topLeftCell="A129" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="B147" sqref="B147"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="23.5" x14ac:dyDescent="0.55000000000000004"/>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="23.25" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="3.90625" customWidth="1"/>
-    <col min="2" max="2" width="77.36328125" customWidth="1"/>
-    <col min="3" max="3" width="16.1796875" customWidth="1"/>
-    <col min="4" max="4" width="16.453125" style="423" customWidth="1"/>
+    <col min="1" max="1" width="3.85546875" customWidth="1"/>
+    <col min="2" max="2" width="77.42578125" customWidth="1"/>
+    <col min="3" max="3" width="16.140625" customWidth="1"/>
+    <col min="4" max="4" width="16.42578125" style="423" customWidth="1"/>
     <col min="5" max="5" width="15" customWidth="1"/>
-    <col min="6" max="6" width="13.453125" style="249" customWidth="1"/>
-    <col min="7" max="7" width="17.453125" hidden="1" customWidth="1"/>
-    <col min="8" max="8" width="9.90625" hidden="1" customWidth="1"/>
-    <col min="9" max="13" width="13.36328125" hidden="1" customWidth="1"/>
+    <col min="6" max="6" width="13.42578125" style="249" customWidth="1"/>
+    <col min="7" max="7" width="17.42578125" hidden="1" customWidth="1"/>
+    <col min="8" max="8" width="9.85546875" hidden="1" customWidth="1"/>
+    <col min="9" max="13" width="13.42578125" hidden="1" customWidth="1"/>
     <col min="14" max="14" width="5" hidden="1" customWidth="1"/>
-    <col min="15" max="15" width="15.6328125" hidden="1" customWidth="1"/>
-    <col min="16" max="16" width="12.54296875" hidden="1" customWidth="1"/>
+    <col min="15" max="15" width="15.5703125" hidden="1" customWidth="1"/>
+    <col min="16" max="16" width="12.5703125" hidden="1" customWidth="1"/>
     <col min="17" max="17" width="9" hidden="1" customWidth="1"/>
-    <col min="18" max="18" width="18.6328125" customWidth="1"/>
-    <col min="19" max="19" width="18.6328125" hidden="1" customWidth="1"/>
-    <col min="20" max="20" width="9.453125" hidden="1" customWidth="1"/>
+    <col min="18" max="18" width="18.5703125" customWidth="1"/>
+    <col min="19" max="19" width="18.5703125" hidden="1" customWidth="1"/>
+    <col min="20" max="20" width="9.42578125" hidden="1" customWidth="1"/>
     <col min="21" max="21" width="11" hidden="1" customWidth="1"/>
-    <col min="22" max="22" width="7.6328125" hidden="1" customWidth="1"/>
-    <col min="23" max="23" width="10.54296875" hidden="1" customWidth="1"/>
-    <col min="24" max="24" width="5.6328125" hidden="1" customWidth="1"/>
-    <col min="25" max="25" width="15.6328125" hidden="1" customWidth="1"/>
-    <col min="26" max="26" width="12.54296875" hidden="1" customWidth="1"/>
+    <col min="22" max="22" width="7.5703125" hidden="1" customWidth="1"/>
+    <col min="23" max="23" width="10.5703125" hidden="1" customWidth="1"/>
+    <col min="24" max="24" width="5.5703125" hidden="1" customWidth="1"/>
+    <col min="25" max="25" width="15.5703125" hidden="1" customWidth="1"/>
+    <col min="26" max="26" width="12.5703125" hidden="1" customWidth="1"/>
     <col min="27" max="27" width="9" hidden="1" customWidth="1"/>
-    <col min="28" max="28" width="18.6328125" customWidth="1"/>
-    <col min="29" max="29" width="18.6328125" hidden="1" customWidth="1"/>
-    <col min="30" max="30" width="9.453125" hidden="1" customWidth="1"/>
+    <col min="28" max="28" width="18.5703125" customWidth="1"/>
+    <col min="29" max="29" width="18.5703125" hidden="1" customWidth="1"/>
+    <col min="30" max="30" width="9.42578125" hidden="1" customWidth="1"/>
     <col min="31" max="31" width="11" hidden="1" customWidth="1"/>
-    <col min="32" max="32" width="9.6328125" hidden="1" customWidth="1"/>
-    <col min="33" max="33" width="9.08984375" hidden="1" customWidth="1"/>
-    <col min="34" max="34" width="5.6328125" hidden="1" customWidth="1"/>
-    <col min="35" max="35" width="85.6328125" style="200" hidden="1" customWidth="1"/>
-    <col min="36" max="36" width="5.36328125" hidden="1" customWidth="1"/>
+    <col min="32" max="32" width="9.5703125" hidden="1" customWidth="1"/>
+    <col min="33" max="33" width="9.140625" hidden="1" customWidth="1"/>
+    <col min="34" max="34" width="5.5703125" hidden="1" customWidth="1"/>
+    <col min="35" max="35" width="85.5703125" style="200" hidden="1" customWidth="1"/>
+    <col min="36" max="36" width="5.42578125" hidden="1" customWidth="1"/>
     <col min="37" max="37" width="13" hidden="1" customWidth="1"/>
-    <col min="38" max="38" width="11.90625" hidden="1" customWidth="1"/>
-    <col min="39" max="39" width="9.6328125" hidden="1" customWidth="1"/>
-    <col min="40" max="40" width="17.6328125" bestFit="1" customWidth="1"/>
+    <col min="38" max="38" width="11.85546875" hidden="1" customWidth="1"/>
+    <col min="39" max="39" width="9.5703125" hidden="1" customWidth="1"/>
+    <col min="40" max="40" width="17.5703125" bestFit="1" customWidth="1"/>
     <col min="41" max="41" width="13" hidden="1" customWidth="1"/>
-    <col min="42" max="42" width="10.36328125" hidden="1" customWidth="1"/>
-    <col min="43" max="43" width="8.90625" hidden="1" customWidth="1"/>
-    <col min="44" max="44" width="8.36328125" hidden="1" customWidth="1"/>
-    <col min="45" max="45" width="10.54296875" hidden="1" customWidth="1"/>
-    <col min="46" max="46" width="5.6328125" hidden="1" customWidth="1"/>
-    <col min="47" max="47" width="14.90625" hidden="1" customWidth="1"/>
-    <col min="48" max="48" width="16.36328125" hidden="1" customWidth="1"/>
-    <col min="49" max="49" width="12.453125" hidden="1" customWidth="1"/>
-    <col min="50" max="50" width="17.6328125" bestFit="1" customWidth="1"/>
-    <col min="51" max="51" width="7.6328125" hidden="1" customWidth="1"/>
-    <col min="52" max="52" width="9.6328125" hidden="1" customWidth="1"/>
-    <col min="53" max="53" width="8.90625" hidden="1" customWidth="1"/>
-    <col min="54" max="54" width="8.36328125" hidden="1" customWidth="1"/>
-    <col min="55" max="55" width="8.54296875" hidden="1" customWidth="1"/>
-    <col min="56" max="56" width="5.6328125" hidden="1" customWidth="1"/>
+    <col min="42" max="42" width="10.42578125" hidden="1" customWidth="1"/>
+    <col min="43" max="43" width="8.85546875" hidden="1" customWidth="1"/>
+    <col min="44" max="44" width="8.42578125" hidden="1" customWidth="1"/>
+    <col min="45" max="45" width="10.5703125" hidden="1" customWidth="1"/>
+    <col min="46" max="46" width="5.5703125" hidden="1" customWidth="1"/>
+    <col min="47" max="47" width="14.85546875" hidden="1" customWidth="1"/>
+    <col min="48" max="48" width="16.42578125" hidden="1" customWidth="1"/>
+    <col min="49" max="49" width="12.42578125" hidden="1" customWidth="1"/>
+    <col min="50" max="50" width="17.5703125" bestFit="1" customWidth="1"/>
+    <col min="51" max="51" width="7.5703125" hidden="1" customWidth="1"/>
+    <col min="52" max="52" width="9.5703125" hidden="1" customWidth="1"/>
+    <col min="53" max="53" width="8.85546875" hidden="1" customWidth="1"/>
+    <col min="54" max="54" width="8.42578125" hidden="1" customWidth="1"/>
+    <col min="55" max="55" width="8.5703125" hidden="1" customWidth="1"/>
+    <col min="56" max="56" width="5.5703125" hidden="1" customWidth="1"/>
     <col min="57" max="57" width="13" hidden="1" customWidth="1"/>
-    <col min="58" max="58" width="16.36328125" hidden="1" customWidth="1"/>
-    <col min="59" max="59" width="9.6328125" hidden="1" customWidth="1"/>
-    <col min="60" max="60" width="19.08984375" customWidth="1"/>
-    <col min="61" max="61" width="19.08984375" hidden="1" customWidth="1"/>
-    <col min="62" max="62" width="8.08984375" hidden="1" customWidth="1"/>
-    <col min="63" max="65" width="8.54296875" hidden="1" customWidth="1"/>
+    <col min="58" max="58" width="16.42578125" hidden="1" customWidth="1"/>
+    <col min="59" max="59" width="9.5703125" hidden="1" customWidth="1"/>
+    <col min="60" max="60" width="19.140625" customWidth="1"/>
+    <col min="61" max="61" width="19.140625" hidden="1" customWidth="1"/>
+    <col min="62" max="62" width="8.140625" hidden="1" customWidth="1"/>
+    <col min="63" max="65" width="8.5703125" hidden="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:65" ht="103.5" customHeight="1" x14ac:dyDescent="0.55000000000000004"/>
-    <row r="2" spans="1:65" s="108" customFormat="1" ht="46" x14ac:dyDescent="1">
+    <row r="1" spans="1:65" ht="103.5" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="2" spans="1:65" s="108" customFormat="1" ht="46.5" x14ac:dyDescent="0.7">
       <c r="B2" s="108" t="s">
         <v>151</v>
       </c>
@@ -3560,7 +3563,7 @@
       <c r="F2" s="249"/>
       <c r="AI2" s="201"/>
     </row>
-    <row r="3" spans="1:65" s="108" customFormat="1" ht="17.25" hidden="1" customHeight="1" x14ac:dyDescent="1">
+    <row r="3" spans="1:65" s="108" customFormat="1" ht="17.25" hidden="1" customHeight="1" x14ac:dyDescent="0.7">
       <c r="A3" s="189"/>
       <c r="B3" s="189"/>
       <c r="C3" s="189"/>
@@ -3627,7 +3630,7 @@
       <c r="BL3" s="189"/>
       <c r="BM3" s="189"/>
     </row>
-    <row r="4" spans="1:65" s="189" customFormat="1" hidden="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="4" spans="1:65" s="189" customFormat="1" hidden="1" x14ac:dyDescent="0.35">
       <c r="B4" s="190" t="s">
         <v>57</v>
       </c>
@@ -3640,7 +3643,7 @@
       <c r="I4" s="190"/>
       <c r="AI4" s="202"/>
     </row>
-    <row r="5" spans="1:65" s="189" customFormat="1" hidden="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="5" spans="1:65" s="189" customFormat="1" hidden="1" x14ac:dyDescent="0.35">
       <c r="B5" s="192" t="s">
         <v>58</v>
       </c>
@@ -3667,7 +3670,7 @@
       </c>
       <c r="AI5" s="202"/>
     </row>
-    <row r="6" spans="1:65" s="189" customFormat="1" hidden="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="6" spans="1:65" s="189" customFormat="1" hidden="1" x14ac:dyDescent="0.35">
       <c r="B6" s="192" t="s">
         <v>59</v>
       </c>
@@ -3694,7 +3697,7 @@
       </c>
       <c r="AI6" s="202"/>
     </row>
-    <row r="7" spans="1:65" s="189" customFormat="1" hidden="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="7" spans="1:65" s="189" customFormat="1" hidden="1" x14ac:dyDescent="0.35">
       <c r="B7" s="193"/>
       <c r="C7" s="194"/>
       <c r="D7" s="428"/>
@@ -3704,7 +3707,7 @@
       <c r="H7" s="194"/>
       <c r="AI7" s="202"/>
     </row>
-    <row r="8" spans="1:65" s="189" customFormat="1" hidden="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="8" spans="1:65" s="189" customFormat="1" hidden="1" x14ac:dyDescent="0.35">
       <c r="B8" s="190" t="s">
         <v>69</v>
       </c>
@@ -3717,7 +3720,7 @@
       <c r="I8" s="190"/>
       <c r="AI8" s="202"/>
     </row>
-    <row r="9" spans="1:65" s="189" customFormat="1" hidden="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="9" spans="1:65" s="189" customFormat="1" hidden="1" x14ac:dyDescent="0.35">
       <c r="B9" s="192" t="s">
         <v>58</v>
       </c>
@@ -3738,7 +3741,7 @@
       </c>
       <c r="AI9" s="202"/>
     </row>
-    <row r="10" spans="1:65" s="189" customFormat="1" ht="22.5" hidden="1" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="10" spans="1:65" s="189" customFormat="1" ht="22.5" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B10" s="192" t="s">
         <v>64</v>
       </c>
@@ -3759,7 +3762,7 @@
       </c>
       <c r="AI10" s="202"/>
     </row>
-    <row r="11" spans="1:65" s="189" customFormat="1" ht="19.5" hidden="1" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="11" spans="1:65" s="189" customFormat="1" ht="19.5" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B11" s="196"/>
       <c r="C11" s="197"/>
       <c r="D11" s="428"/>
@@ -3774,7 +3777,7 @@
       <c r="M11" s="202"/>
       <c r="AI11" s="202"/>
     </row>
-    <row r="12" spans="1:65" s="189" customFormat="1" ht="24" thickBot="1" x14ac:dyDescent="0.6">
+    <row r="12" spans="1:65" s="189" customFormat="1" ht="24" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B12" s="196"/>
       <c r="C12" s="197"/>
       <c r="D12" s="428"/>
@@ -3789,7 +3792,7 @@
       <c r="M12" s="202"/>
       <c r="AI12" s="202"/>
     </row>
-    <row r="13" spans="1:65" ht="24" thickBot="1" x14ac:dyDescent="0.6">
+    <row r="13" spans="1:65" ht="24" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A13" s="90"/>
       <c r="B13" s="25"/>
       <c r="C13" s="114"/>
@@ -3878,7 +3881,7 @@
       <c r="BL13" s="234"/>
       <c r="BM13" s="242"/>
     </row>
-    <row r="14" spans="1:65" ht="24" thickBot="1" x14ac:dyDescent="0.6">
+    <row r="14" spans="1:65" ht="24" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A14" s="91"/>
       <c r="B14" s="40"/>
       <c r="C14" s="92" t="s">
@@ -3975,7 +3978,7 @@
       <c r="BL14" s="240"/>
       <c r="BM14" s="153"/>
     </row>
-    <row r="15" spans="1:65" s="1" customFormat="1" ht="21.5" thickBot="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="15" spans="1:65" s="1" customFormat="1" ht="21.75" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A15" s="94" t="s">
         <v>0</v>
       </c>
@@ -4156,7 +4159,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="16" spans="1:65" s="226" customFormat="1" ht="28.5" x14ac:dyDescent="0.65">
+    <row r="16" spans="1:65" s="226" customFormat="1" ht="28.5" x14ac:dyDescent="0.45">
       <c r="A16" s="211"/>
       <c r="B16" s="212" t="s">
         <v>158</v>
@@ -4246,7 +4249,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="17" spans="1:68" s="226" customFormat="1" ht="28.5" x14ac:dyDescent="0.65">
+    <row r="17" spans="1:68" s="226" customFormat="1" ht="28.5" x14ac:dyDescent="0.45">
       <c r="A17" s="310"/>
       <c r="B17" s="327" t="s">
         <v>157</v>
@@ -4315,7 +4318,7 @@
       <c r="BL17" s="214"/>
       <c r="BM17" s="213"/>
     </row>
-    <row r="18" spans="1:68" x14ac:dyDescent="0.55000000000000004">
+    <row r="18" spans="1:68" x14ac:dyDescent="0.35">
       <c r="A18" s="95"/>
       <c r="B18" s="19" t="s">
         <v>211</v>
@@ -4523,7 +4526,7 @@
       <c r="BL18" s="267"/>
       <c r="BM18" s="264"/>
     </row>
-    <row r="19" spans="1:68" x14ac:dyDescent="0.55000000000000004">
+    <row r="19" spans="1:68" x14ac:dyDescent="0.35">
       <c r="A19" s="95"/>
       <c r="B19" s="404" t="s">
         <v>272</v>
@@ -4731,7 +4734,7 @@
       <c r="BL19" s="267"/>
       <c r="BM19" s="264"/>
     </row>
-    <row r="20" spans="1:68" x14ac:dyDescent="0.55000000000000004">
+    <row r="20" spans="1:68" x14ac:dyDescent="0.35">
       <c r="A20" s="95"/>
       <c r="B20" s="404" t="s">
         <v>255</v>
@@ -4939,7 +4942,7 @@
       <c r="BL20" s="267"/>
       <c r="BM20" s="264"/>
     </row>
-    <row r="21" spans="1:68" x14ac:dyDescent="0.55000000000000004">
+    <row r="21" spans="1:68" x14ac:dyDescent="0.35">
       <c r="A21" s="95"/>
       <c r="B21" s="19" t="s">
         <v>202</v>
@@ -5132,7 +5135,7 @@
       <c r="BL21" s="267"/>
       <c r="BM21" s="264"/>
     </row>
-    <row r="22" spans="1:68" x14ac:dyDescent="0.55000000000000004">
+    <row r="22" spans="1:68" x14ac:dyDescent="0.35">
       <c r="A22" s="95"/>
       <c r="B22" s="19" t="s">
         <v>203</v>
@@ -5340,7 +5343,7 @@
       <c r="BL22" s="267"/>
       <c r="BM22" s="264"/>
     </row>
-    <row r="23" spans="1:68" x14ac:dyDescent="0.55000000000000004">
+    <row r="23" spans="1:68" x14ac:dyDescent="0.35">
       <c r="A23" s="95"/>
       <c r="B23" s="19" t="s">
         <v>204</v>
@@ -5554,7 +5557,7 @@
         <v>455</v>
       </c>
     </row>
-    <row r="24" spans="1:68" x14ac:dyDescent="0.55000000000000004">
+    <row r="24" spans="1:68" x14ac:dyDescent="0.35">
       <c r="A24" s="95"/>
       <c r="B24" s="19" t="s">
         <v>205</v>
@@ -5762,7 +5765,7 @@
       <c r="BL24" s="267"/>
       <c r="BM24" s="264"/>
     </row>
-    <row r="25" spans="1:68" x14ac:dyDescent="0.55000000000000004">
+    <row r="25" spans="1:68" x14ac:dyDescent="0.35">
       <c r="A25" s="95"/>
       <c r="B25" s="19" t="s">
         <v>148</v>
@@ -5962,7 +5965,7 @@
       <c r="BL25" s="267"/>
       <c r="BM25" s="264"/>
     </row>
-    <row r="26" spans="1:68" x14ac:dyDescent="0.55000000000000004">
+    <row r="26" spans="1:68" x14ac:dyDescent="0.35">
       <c r="A26" s="95"/>
       <c r="B26" s="247"/>
       <c r="C26" s="259"/>
@@ -6155,7 +6158,7 @@
       <c r="BL26" s="267"/>
       <c r="BM26" s="264"/>
     </row>
-    <row r="27" spans="1:68" s="226" customFormat="1" ht="28.5" x14ac:dyDescent="0.65">
+    <row r="27" spans="1:68" s="226" customFormat="1" ht="28.5" x14ac:dyDescent="0.45">
       <c r="A27" s="310"/>
       <c r="B27" s="327" t="s">
         <v>159</v>
@@ -6224,7 +6227,7 @@
       <c r="BL27" s="214"/>
       <c r="BM27" s="213"/>
     </row>
-    <row r="28" spans="1:68" x14ac:dyDescent="0.55000000000000004">
+    <row r="28" spans="1:68" x14ac:dyDescent="0.35">
       <c r="A28" s="95"/>
       <c r="B28" s="308" t="s">
         <v>133</v>
@@ -6432,7 +6435,7 @@
         <v/>
       </c>
     </row>
-    <row r="29" spans="1:68" x14ac:dyDescent="0.55000000000000004">
+    <row r="29" spans="1:68" x14ac:dyDescent="0.35">
       <c r="A29" s="95"/>
       <c r="B29" s="454" t="s">
         <v>303</v>
@@ -6640,7 +6643,7 @@
         <v/>
       </c>
     </row>
-    <row r="30" spans="1:68" x14ac:dyDescent="0.55000000000000004">
+    <row r="30" spans="1:68" x14ac:dyDescent="0.35">
       <c r="A30" s="95"/>
       <c r="B30" s="19" t="s">
         <v>161</v>
@@ -6833,7 +6836,7 @@
       <c r="BL30" s="50"/>
       <c r="BM30" s="44"/>
     </row>
-    <row r="31" spans="1:68" x14ac:dyDescent="0.55000000000000004">
+    <row r="31" spans="1:68" x14ac:dyDescent="0.35">
       <c r="A31" s="95"/>
       <c r="B31" s="399" t="s">
         <v>248</v>
@@ -7026,7 +7029,7 @@
         <v/>
       </c>
     </row>
-    <row r="32" spans="1:68" x14ac:dyDescent="0.55000000000000004">
+    <row r="32" spans="1:68" x14ac:dyDescent="0.35">
       <c r="A32" s="95"/>
       <c r="B32" s="399" t="s">
         <v>249</v>
@@ -7219,7 +7222,7 @@
         <v/>
       </c>
     </row>
-    <row r="33" spans="1:65" x14ac:dyDescent="0.55000000000000004">
+    <row r="33" spans="1:65" x14ac:dyDescent="0.35">
       <c r="A33" s="95"/>
       <c r="B33" s="399" t="s">
         <v>250</v>
@@ -7412,7 +7415,7 @@
         <v/>
       </c>
     </row>
-    <row r="34" spans="1:65" x14ac:dyDescent="0.55000000000000004">
+    <row r="34" spans="1:65" x14ac:dyDescent="0.35">
       <c r="A34" s="95"/>
       <c r="B34" s="396" t="s">
         <v>162</v>
@@ -7605,7 +7608,7 @@
         <v/>
       </c>
     </row>
-    <row r="35" spans="1:65" x14ac:dyDescent="0.55000000000000004">
+    <row r="35" spans="1:65" x14ac:dyDescent="0.35">
       <c r="A35" s="95"/>
       <c r="B35" s="453" t="s">
         <v>297</v>
@@ -7798,7 +7801,7 @@
         <v/>
       </c>
     </row>
-    <row r="36" spans="1:65" x14ac:dyDescent="0.55000000000000004">
+    <row r="36" spans="1:65" x14ac:dyDescent="0.35">
       <c r="A36" s="95"/>
       <c r="B36" s="452" t="s">
         <v>267</v>
@@ -7991,7 +7994,7 @@
         <v/>
       </c>
     </row>
-    <row r="37" spans="1:65" x14ac:dyDescent="0.55000000000000004">
+    <row r="37" spans="1:65" x14ac:dyDescent="0.35">
       <c r="A37" s="95"/>
       <c r="B37" s="452" t="s">
         <v>298</v>
@@ -8184,7 +8187,7 @@
         <v/>
       </c>
     </row>
-    <row r="38" spans="1:65" x14ac:dyDescent="0.55000000000000004">
+    <row r="38" spans="1:65" x14ac:dyDescent="0.35">
       <c r="A38" s="95"/>
       <c r="B38" s="398" t="s">
         <v>268</v>
@@ -8377,7 +8380,7 @@
         <v/>
       </c>
     </row>
-    <row r="39" spans="1:65" x14ac:dyDescent="0.55000000000000004">
+    <row r="39" spans="1:65" x14ac:dyDescent="0.35">
       <c r="A39" s="95"/>
       <c r="B39" s="398" t="s">
         <v>264</v>
@@ -8570,7 +8573,7 @@
         <v/>
       </c>
     </row>
-    <row r="40" spans="1:65" x14ac:dyDescent="0.55000000000000004">
+    <row r="40" spans="1:65" x14ac:dyDescent="0.35">
       <c r="A40" s="95"/>
       <c r="B40" s="439" t="s">
         <v>270</v>
@@ -8763,7 +8766,7 @@
         <v/>
       </c>
     </row>
-    <row r="41" spans="1:65" x14ac:dyDescent="0.55000000000000004">
+    <row r="41" spans="1:65" x14ac:dyDescent="0.35">
       <c r="A41" s="95"/>
       <c r="B41" s="439" t="s">
         <v>309</v>
@@ -8956,7 +8959,7 @@
         <v/>
       </c>
     </row>
-    <row r="42" spans="1:65" x14ac:dyDescent="0.55000000000000004">
+    <row r="42" spans="1:65" x14ac:dyDescent="0.35">
       <c r="A42" s="95"/>
       <c r="B42" s="439" t="s">
         <v>262</v>
@@ -9149,7 +9152,7 @@
         <v/>
       </c>
     </row>
-    <row r="43" spans="1:65" x14ac:dyDescent="0.55000000000000004">
+    <row r="43" spans="1:65" x14ac:dyDescent="0.35">
       <c r="A43" s="95"/>
       <c r="B43" s="437" t="s">
         <v>263</v>
@@ -9342,7 +9345,7 @@
         <v/>
       </c>
     </row>
-    <row r="44" spans="1:65" x14ac:dyDescent="0.55000000000000004">
+    <row r="44" spans="1:65" x14ac:dyDescent="0.35">
       <c r="A44" s="95"/>
       <c r="B44" s="440" t="s">
         <v>269</v>
@@ -9535,7 +9538,7 @@
         <v/>
       </c>
     </row>
-    <row r="45" spans="1:65" x14ac:dyDescent="0.55000000000000004">
+    <row r="45" spans="1:65" x14ac:dyDescent="0.35">
       <c r="A45" s="95"/>
       <c r="B45" s="440" t="s">
         <v>265</v>
@@ -9728,7 +9731,7 @@
         <v/>
       </c>
     </row>
-    <row r="46" spans="1:65" x14ac:dyDescent="0.55000000000000004">
+    <row r="46" spans="1:65" x14ac:dyDescent="0.35">
       <c r="A46" s="95"/>
       <c r="B46" s="440" t="s">
         <v>283</v>
@@ -9921,7 +9924,7 @@
         <v/>
       </c>
     </row>
-    <row r="47" spans="1:65" x14ac:dyDescent="0.55000000000000004">
+    <row r="47" spans="1:65" x14ac:dyDescent="0.35">
       <c r="A47" s="95"/>
       <c r="B47" s="449" t="s">
         <v>271</v>
@@ -10114,7 +10117,7 @@
         <v/>
       </c>
     </row>
-    <row r="48" spans="1:65" x14ac:dyDescent="0.55000000000000004">
+    <row r="48" spans="1:65" x14ac:dyDescent="0.35">
       <c r="A48" s="95"/>
       <c r="B48" s="339" t="s">
         <v>257</v>
@@ -10307,7 +10310,7 @@
         <v/>
       </c>
     </row>
-    <row r="49" spans="1:69" x14ac:dyDescent="0.55000000000000004">
+    <row r="49" spans="1:69" x14ac:dyDescent="0.35">
       <c r="A49" s="95"/>
       <c r="B49" s="437" t="s">
         <v>261</v>
@@ -10500,7 +10503,7 @@
         <v/>
       </c>
     </row>
-    <row r="50" spans="1:69" x14ac:dyDescent="0.55000000000000004">
+    <row r="50" spans="1:69" x14ac:dyDescent="0.35">
       <c r="A50" s="95"/>
       <c r="B50" s="440" t="s">
         <v>282</v>
@@ -10693,7 +10696,7 @@
         <v/>
       </c>
     </row>
-    <row r="51" spans="1:69" x14ac:dyDescent="0.55000000000000004">
+    <row r="51" spans="1:69" x14ac:dyDescent="0.35">
       <c r="A51" s="95"/>
       <c r="B51" s="396" t="s">
         <v>243</v>
@@ -10886,7 +10889,7 @@
         <v/>
       </c>
     </row>
-    <row r="52" spans="1:69" x14ac:dyDescent="0.55000000000000004">
+    <row r="52" spans="1:69" x14ac:dyDescent="0.35">
       <c r="A52" s="401"/>
       <c r="B52" s="396" t="s">
         <v>251</v>
@@ -11079,7 +11082,7 @@
         <v/>
       </c>
     </row>
-    <row r="53" spans="1:69" x14ac:dyDescent="0.55000000000000004">
+    <row r="53" spans="1:69" x14ac:dyDescent="0.35">
       <c r="A53" s="95"/>
       <c r="B53" s="269" t="s">
         <v>206</v>
@@ -11242,7 +11245,7 @@
       <c r="BL53" s="50"/>
       <c r="BM53" s="44"/>
     </row>
-    <row r="54" spans="1:69" x14ac:dyDescent="0.55000000000000004">
+    <row r="54" spans="1:69" x14ac:dyDescent="0.35">
       <c r="A54" s="95"/>
       <c r="B54" s="308" t="s">
         <v>207</v>
@@ -11402,7 +11405,7 @@
       <c r="BL54" s="50"/>
       <c r="BM54" s="44"/>
     </row>
-    <row r="55" spans="1:69" x14ac:dyDescent="0.55000000000000004">
+    <row r="55" spans="1:69" x14ac:dyDescent="0.35">
       <c r="A55" s="95"/>
       <c r="B55" s="19" t="s">
         <v>163</v>
@@ -11583,7 +11586,7 @@
         <v>2.2999999999999998</v>
       </c>
     </row>
-    <row r="56" spans="1:69" x14ac:dyDescent="0.55000000000000004">
+    <row r="56" spans="1:69" x14ac:dyDescent="0.35">
       <c r="A56" s="95"/>
       <c r="B56" s="19" t="s">
         <v>167</v>
@@ -11776,7 +11779,7 @@
         <v/>
       </c>
     </row>
-    <row r="57" spans="1:69" x14ac:dyDescent="0.55000000000000004">
+    <row r="57" spans="1:69" x14ac:dyDescent="0.35">
       <c r="A57" s="95"/>
       <c r="B57" s="397" t="s">
         <v>164</v>
@@ -11954,7 +11957,7 @@
       <c r="BL57" s="50"/>
       <c r="BM57" s="44"/>
     </row>
-    <row r="58" spans="1:69" x14ac:dyDescent="0.55000000000000004">
+    <row r="58" spans="1:69" x14ac:dyDescent="0.35">
       <c r="A58" s="95"/>
       <c r="B58" s="397" t="s">
         <v>244</v>
@@ -12132,7 +12135,7 @@
       <c r="BL58" s="50"/>
       <c r="BM58" s="44"/>
     </row>
-    <row r="59" spans="1:69" x14ac:dyDescent="0.55000000000000004">
+    <row r="59" spans="1:69" x14ac:dyDescent="0.35">
       <c r="A59" s="95"/>
       <c r="B59" s="397" t="s">
         <v>258</v>
@@ -12310,7 +12313,7 @@
       <c r="BL59" s="50"/>
       <c r="BM59" s="44"/>
     </row>
-    <row r="60" spans="1:69" x14ac:dyDescent="0.55000000000000004">
+    <row r="60" spans="1:69" x14ac:dyDescent="0.35">
       <c r="A60" s="95"/>
       <c r="B60" s="398" t="s">
         <v>245</v>
@@ -12488,7 +12491,7 @@
       <c r="BL60" s="50"/>
       <c r="BM60" s="44"/>
     </row>
-    <row r="61" spans="1:69" x14ac:dyDescent="0.55000000000000004">
+    <row r="61" spans="1:69" x14ac:dyDescent="0.35">
       <c r="A61" s="95"/>
       <c r="B61" s="398" t="s">
         <v>246</v>
@@ -12666,7 +12669,7 @@
       <c r="BL61" s="50"/>
       <c r="BM61" s="44"/>
     </row>
-    <row r="62" spans="1:69" x14ac:dyDescent="0.55000000000000004">
+    <row r="62" spans="1:69" x14ac:dyDescent="0.35">
       <c r="A62" s="95"/>
       <c r="B62" s="339" t="s">
         <v>165</v>
@@ -12844,7 +12847,7 @@
       <c r="BL62" s="50"/>
       <c r="BM62" s="44"/>
     </row>
-    <row r="63" spans="1:69" x14ac:dyDescent="0.55000000000000004">
+    <row r="63" spans="1:69" x14ac:dyDescent="0.35">
       <c r="A63" s="95"/>
       <c r="B63" s="308" t="s">
         <v>132</v>
@@ -13025,7 +13028,7 @@
       <c r="BL63" s="50"/>
       <c r="BM63" s="44"/>
     </row>
-    <row r="64" spans="1:69" x14ac:dyDescent="0.55000000000000004">
+    <row r="64" spans="1:69" x14ac:dyDescent="0.35">
       <c r="A64" s="95"/>
       <c r="B64" s="19" t="s">
         <v>166</v>
@@ -13203,7 +13206,7 @@
       <c r="BL64" s="50"/>
       <c r="BM64" s="44"/>
     </row>
-    <row r="65" spans="1:65" x14ac:dyDescent="0.55000000000000004">
+    <row r="65" spans="1:65" x14ac:dyDescent="0.35">
       <c r="A65" s="95"/>
       <c r="B65" s="308" t="s">
         <v>168</v>
@@ -13411,7 +13414,7 @@
         <v/>
       </c>
     </row>
-    <row r="66" spans="1:65" x14ac:dyDescent="0.55000000000000004">
+    <row r="66" spans="1:65" x14ac:dyDescent="0.35">
       <c r="A66" s="95"/>
       <c r="B66" s="269" t="s">
         <v>169</v>
@@ -13619,7 +13622,7 @@
         <v>1.5398353800161703E+28</v>
       </c>
     </row>
-    <row r="67" spans="1:65" x14ac:dyDescent="0.55000000000000004">
+    <row r="67" spans="1:65" x14ac:dyDescent="0.35">
       <c r="A67" s="95"/>
       <c r="B67" s="436" t="s">
         <v>260</v>
@@ -13827,7 +13830,7 @@
         <v>1.142978900832057E+29</v>
       </c>
     </row>
-    <row r="68" spans="1:65" x14ac:dyDescent="0.55000000000000004">
+    <row r="68" spans="1:65" x14ac:dyDescent="0.35">
       <c r="A68" s="95"/>
       <c r="B68" s="436" t="s">
         <v>259</v>
@@ -14035,7 +14038,7 @@
         <v>3.248207164759231E+28</v>
       </c>
     </row>
-    <row r="69" spans="1:65" x14ac:dyDescent="0.55000000000000004">
+    <row r="69" spans="1:65" x14ac:dyDescent="0.35">
       <c r="A69" s="95"/>
       <c r="B69" s="446" t="s">
         <v>280</v>
@@ -14217,7 +14220,7 @@
       <c r="BL69" s="340"/>
       <c r="BM69" s="34"/>
     </row>
-    <row r="70" spans="1:65" x14ac:dyDescent="0.55000000000000004">
+    <row r="70" spans="1:65" x14ac:dyDescent="0.35">
       <c r="A70" s="95"/>
       <c r="B70" s="447" t="s">
         <v>281</v>
@@ -14399,7 +14402,7 @@
       <c r="BL70" s="340"/>
       <c r="BM70" s="34"/>
     </row>
-    <row r="71" spans="1:65" x14ac:dyDescent="0.55000000000000004">
+    <row r="71" spans="1:65" x14ac:dyDescent="0.35">
       <c r="A71" s="95"/>
       <c r="B71" s="341" t="s">
         <v>286</v>
@@ -14581,7 +14584,7 @@
       <c r="BL71" s="340"/>
       <c r="BM71" s="34"/>
     </row>
-    <row r="72" spans="1:65" x14ac:dyDescent="0.55000000000000004">
+    <row r="72" spans="1:65" x14ac:dyDescent="0.35">
       <c r="A72" s="95"/>
       <c r="B72" s="341" t="s">
         <v>209</v>
@@ -14763,7 +14766,7 @@
       <c r="BL72" s="340"/>
       <c r="BM72" s="34"/>
     </row>
-    <row r="73" spans="1:65" x14ac:dyDescent="0.55000000000000004">
+    <row r="73" spans="1:65" x14ac:dyDescent="0.35">
       <c r="A73" s="95"/>
       <c r="B73" s="403" t="s">
         <v>241</v>
@@ -14971,7 +14974,7 @@
         <v/>
       </c>
     </row>
-    <row r="74" spans="1:65" x14ac:dyDescent="0.55000000000000004">
+    <row r="74" spans="1:65" x14ac:dyDescent="0.35">
       <c r="A74" s="95"/>
       <c r="B74" s="450" t="s">
         <v>292</v>
@@ -15179,7 +15182,7 @@
         <v/>
       </c>
     </row>
-    <row r="75" spans="1:65" x14ac:dyDescent="0.55000000000000004">
+    <row r="75" spans="1:65" x14ac:dyDescent="0.35">
       <c r="A75" s="95"/>
       <c r="B75" s="450" t="s">
         <v>291</v>
@@ -15387,7 +15390,7 @@
         <v/>
       </c>
     </row>
-    <row r="76" spans="1:65" x14ac:dyDescent="0.55000000000000004">
+    <row r="76" spans="1:65" x14ac:dyDescent="0.35">
       <c r="A76" s="95"/>
       <c r="B76" s="450" t="s">
         <v>289</v>
@@ -15595,7 +15598,7 @@
         <v/>
       </c>
     </row>
-    <row r="77" spans="1:65" x14ac:dyDescent="0.55000000000000004">
+    <row r="77" spans="1:65" x14ac:dyDescent="0.35">
       <c r="A77" s="95"/>
       <c r="B77" s="450" t="s">
         <v>254</v>
@@ -15803,7 +15806,7 @@
         <v/>
       </c>
     </row>
-    <row r="78" spans="1:65" x14ac:dyDescent="0.55000000000000004">
+    <row r="78" spans="1:65" x14ac:dyDescent="0.35">
       <c r="A78" s="95"/>
       <c r="B78" s="308" t="s">
         <v>247</v>
@@ -16011,7 +16014,7 @@
         <v/>
       </c>
     </row>
-    <row r="79" spans="1:65" x14ac:dyDescent="0.55000000000000004">
+    <row r="79" spans="1:65" x14ac:dyDescent="0.35">
       <c r="A79" s="95"/>
       <c r="B79" s="400" t="s">
         <v>296</v>
@@ -16219,7 +16222,7 @@
         <v/>
       </c>
     </row>
-    <row r="80" spans="1:65" x14ac:dyDescent="0.55000000000000004">
+    <row r="80" spans="1:65" x14ac:dyDescent="0.35">
       <c r="A80" s="95"/>
       <c r="B80" s="339" t="s">
         <v>295</v>
@@ -16427,7 +16430,7 @@
         <v/>
       </c>
     </row>
-    <row r="81" spans="1:65" x14ac:dyDescent="0.55000000000000004">
+    <row r="81" spans="1:65" x14ac:dyDescent="0.35">
       <c r="A81" s="95"/>
       <c r="B81" s="339" t="s">
         <v>252</v>
@@ -16635,7 +16638,7 @@
         <v/>
       </c>
     </row>
-    <row r="82" spans="1:65" x14ac:dyDescent="0.55000000000000004">
+    <row r="82" spans="1:65" x14ac:dyDescent="0.35">
       <c r="A82" s="95"/>
       <c r="B82" s="339" t="s">
         <v>253</v>
@@ -16843,7 +16846,7 @@
         <v/>
       </c>
     </row>
-    <row r="83" spans="1:65" x14ac:dyDescent="0.55000000000000004">
+    <row r="83" spans="1:65" x14ac:dyDescent="0.35">
       <c r="A83" s="95"/>
       <c r="B83" s="19" t="s">
         <v>288</v>
@@ -17009,7 +17012,7 @@
       <c r="BL83" s="50"/>
       <c r="BM83" s="44"/>
     </row>
-    <row r="84" spans="1:65" x14ac:dyDescent="0.55000000000000004">
+    <row r="84" spans="1:65" x14ac:dyDescent="0.35">
       <c r="A84" s="95"/>
       <c r="B84" s="339" t="s">
         <v>294</v>
@@ -17175,7 +17178,7 @@
       <c r="BL84" s="50"/>
       <c r="BM84" s="44"/>
     </row>
-    <row r="85" spans="1:65" x14ac:dyDescent="0.55000000000000004">
+    <row r="85" spans="1:65" x14ac:dyDescent="0.35">
       <c r="A85" s="95"/>
       <c r="B85" s="19" t="s">
         <v>171</v>
@@ -17341,7 +17344,7 @@
       <c r="BL85" s="50"/>
       <c r="BM85" s="44"/>
     </row>
-    <row r="86" spans="1:65" x14ac:dyDescent="0.55000000000000004">
+    <row r="86" spans="1:65" x14ac:dyDescent="0.35">
       <c r="A86" s="95"/>
       <c r="B86" s="19" t="s">
         <v>170</v>
@@ -17576,7 +17579,7 @@
         <v/>
       </c>
     </row>
-    <row r="87" spans="1:65" x14ac:dyDescent="0.55000000000000004">
+    <row r="87" spans="1:65" x14ac:dyDescent="0.35">
       <c r="A87" s="95"/>
       <c r="B87" s="269" t="s">
         <v>210</v>
@@ -17768,7 +17771,7 @@
       <c r="BL87" s="50"/>
       <c r="BM87" s="44"/>
     </row>
-    <row r="88" spans="1:65" x14ac:dyDescent="0.55000000000000004">
+    <row r="88" spans="1:65" x14ac:dyDescent="0.35">
       <c r="A88" s="95"/>
       <c r="B88" s="338" t="s">
         <v>160</v>
@@ -17837,7 +17840,7 @@
       <c r="BL88" s="50"/>
       <c r="BM88" s="44"/>
     </row>
-    <row r="89" spans="1:65" s="226" customFormat="1" ht="28.5" x14ac:dyDescent="0.65">
+    <row r="89" spans="1:65" s="226" customFormat="1" ht="28.5" x14ac:dyDescent="0.45">
       <c r="A89" s="310"/>
       <c r="B89" s="327" t="s">
         <v>149</v>
@@ -17906,7 +17909,7 @@
       <c r="BL89" s="214"/>
       <c r="BM89" s="213"/>
     </row>
-    <row r="90" spans="1:65" x14ac:dyDescent="0.55000000000000004">
+    <row r="90" spans="1:65" x14ac:dyDescent="0.35">
       <c r="A90" s="95"/>
       <c r="B90" s="308" t="s">
         <v>147</v>
@@ -18099,7 +18102,7 @@
       <c r="BL90" s="50"/>
       <c r="BM90" s="44"/>
     </row>
-    <row r="91" spans="1:65" x14ac:dyDescent="0.55000000000000004">
+    <row r="91" spans="1:65" x14ac:dyDescent="0.35">
       <c r="A91" s="95"/>
       <c r="B91" s="308" t="s">
         <v>174</v>
@@ -18292,7 +18295,7 @@
       <c r="BL91" s="50"/>
       <c r="BM91" s="44"/>
     </row>
-    <row r="92" spans="1:65" x14ac:dyDescent="0.55000000000000004">
+    <row r="92" spans="1:65" x14ac:dyDescent="0.35">
       <c r="A92" s="95"/>
       <c r="B92" s="308" t="s">
         <v>173</v>
@@ -18485,7 +18488,7 @@
       <c r="BL92" s="50"/>
       <c r="BM92" s="44"/>
     </row>
-    <row r="93" spans="1:65" x14ac:dyDescent="0.55000000000000004">
+    <row r="93" spans="1:65" x14ac:dyDescent="0.35">
       <c r="A93" s="95"/>
       <c r="B93" s="308" t="s">
         <v>290</v>
@@ -18616,7 +18619,7 @@
       <c r="BL93" s="50"/>
       <c r="BM93" s="44"/>
     </row>
-    <row r="94" spans="1:65" x14ac:dyDescent="0.55000000000000004">
+    <row r="94" spans="1:65" x14ac:dyDescent="0.35">
       <c r="A94" s="95"/>
       <c r="B94" s="308" t="s">
         <v>146</v>
@@ -18747,7 +18750,7 @@
       <c r="BL94" s="50"/>
       <c r="BM94" s="44"/>
     </row>
-    <row r="95" spans="1:65" x14ac:dyDescent="0.55000000000000004">
+    <row r="95" spans="1:65" x14ac:dyDescent="0.35">
       <c r="A95" s="95"/>
       <c r="B95" s="308" t="s">
         <v>172</v>
@@ -18833,7 +18836,7 @@
       <c r="BL95" s="50"/>
       <c r="BM95" s="44"/>
     </row>
-    <row r="96" spans="1:65" x14ac:dyDescent="0.55000000000000004">
+    <row r="96" spans="1:65" x14ac:dyDescent="0.35">
       <c r="A96" s="95"/>
       <c r="B96" s="308" t="s">
         <v>175</v>
@@ -18917,7 +18920,7 @@
       <c r="BL96" s="50"/>
       <c r="BM96" s="44"/>
     </row>
-    <row r="97" spans="1:65" x14ac:dyDescent="0.55000000000000004">
+    <row r="97" spans="1:65" x14ac:dyDescent="0.35">
       <c r="A97" s="95"/>
       <c r="B97" s="308"/>
       <c r="C97" s="259"/>
@@ -18996,7 +18999,7 @@
       <c r="BL97" s="50"/>
       <c r="BM97" s="44"/>
     </row>
-    <row r="98" spans="1:65" x14ac:dyDescent="0.55000000000000004">
+    <row r="98" spans="1:65" x14ac:dyDescent="0.35">
       <c r="A98" s="95"/>
       <c r="B98" s="339" t="s">
         <v>201</v>
@@ -19077,7 +19080,7 @@
       <c r="BL98" s="50"/>
       <c r="BM98" s="44"/>
     </row>
-    <row r="99" spans="1:65" x14ac:dyDescent="0.55000000000000004">
+    <row r="99" spans="1:65" x14ac:dyDescent="0.35">
       <c r="A99" s="95"/>
       <c r="B99" s="269"/>
       <c r="C99" s="259"/>
@@ -19156,7 +19159,7 @@
       <c r="BL99" s="50"/>
       <c r="BM99" s="44"/>
     </row>
-    <row r="100" spans="1:65" s="226" customFormat="1" ht="28.5" x14ac:dyDescent="0.65">
+    <row r="100" spans="1:65" s="226" customFormat="1" ht="28.5" x14ac:dyDescent="0.45">
       <c r="A100" s="310"/>
       <c r="B100" s="327" t="s">
         <v>150</v>
@@ -19237,7 +19240,7 @@
       <c r="BL100" s="214"/>
       <c r="BM100" s="213"/>
     </row>
-    <row r="101" spans="1:65" s="226" customFormat="1" ht="28.5" x14ac:dyDescent="0.65">
+    <row r="101" spans="1:65" s="226" customFormat="1" ht="28.5" x14ac:dyDescent="0.45">
       <c r="A101" s="310"/>
       <c r="B101" s="328" t="s">
         <v>176</v>
@@ -19318,7 +19321,7 @@
       <c r="BL101" s="214"/>
       <c r="BM101" s="213"/>
     </row>
-    <row r="102" spans="1:65" x14ac:dyDescent="0.55000000000000004">
+    <row r="102" spans="1:65" x14ac:dyDescent="0.35">
       <c r="A102" s="95"/>
       <c r="B102" s="19" t="s">
         <v>178</v>
@@ -19478,7 +19481,7 @@
       <c r="BL102" s="50"/>
       <c r="BM102" s="44"/>
     </row>
-    <row r="103" spans="1:65" x14ac:dyDescent="0.55000000000000004">
+    <row r="103" spans="1:65" x14ac:dyDescent="0.35">
       <c r="A103" s="95"/>
       <c r="B103" s="19" t="s">
         <v>177</v>
@@ -19638,7 +19641,7 @@
       <c r="BL103" s="50"/>
       <c r="BM103" s="44"/>
     </row>
-    <row r="104" spans="1:65" x14ac:dyDescent="0.55000000000000004">
+    <row r="104" spans="1:65" x14ac:dyDescent="0.35">
       <c r="A104" s="95"/>
       <c r="B104" s="19" t="s">
         <v>179</v>
@@ -19798,7 +19801,7 @@
       <c r="BL104" s="50"/>
       <c r="BM104" s="44"/>
     </row>
-    <row r="105" spans="1:65" x14ac:dyDescent="0.55000000000000004">
+    <row r="105" spans="1:65" x14ac:dyDescent="0.35">
       <c r="A105" s="95"/>
       <c r="B105" s="19"/>
       <c r="C105" s="259"/>
@@ -19889,7 +19892,7 @@
       <c r="BL105" s="50"/>
       <c r="BM105" s="44"/>
     </row>
-    <row r="106" spans="1:65" s="226" customFormat="1" ht="28.5" x14ac:dyDescent="0.65">
+    <row r="106" spans="1:65" s="226" customFormat="1" ht="28.5" x14ac:dyDescent="0.45">
       <c r="A106" s="310"/>
       <c r="B106" s="328" t="s">
         <v>194</v>
@@ -19958,7 +19961,7 @@
       <c r="BL106" s="214"/>
       <c r="BM106" s="213"/>
     </row>
-    <row r="107" spans="1:65" x14ac:dyDescent="0.55000000000000004">
+    <row r="107" spans="1:65" x14ac:dyDescent="0.35">
       <c r="A107" s="95"/>
       <c r="B107" s="269" t="s">
         <v>180</v>
@@ -20145,7 +20148,7 @@
       <c r="BL107" s="50"/>
       <c r="BM107" s="44"/>
     </row>
-    <row r="108" spans="1:65" x14ac:dyDescent="0.55000000000000004">
+    <row r="108" spans="1:65" x14ac:dyDescent="0.35">
       <c r="A108" s="95"/>
       <c r="B108" s="269" t="s">
         <v>181</v>
@@ -20332,7 +20335,7 @@
       <c r="BL108" s="50"/>
       <c r="BM108" s="44"/>
     </row>
-    <row r="109" spans="1:65" x14ac:dyDescent="0.55000000000000004">
+    <row r="109" spans="1:65" x14ac:dyDescent="0.35">
       <c r="A109" s="95"/>
       <c r="B109" s="269" t="s">
         <v>182</v>
@@ -20467,7 +20470,7 @@
       <c r="BL109" s="50"/>
       <c r="BM109" s="44"/>
     </row>
-    <row r="110" spans="1:65" x14ac:dyDescent="0.55000000000000004">
+    <row r="110" spans="1:65" x14ac:dyDescent="0.35">
       <c r="A110" s="95"/>
       <c r="B110" s="269" t="s">
         <v>183</v>
@@ -20654,7 +20657,7 @@
       <c r="BL110" s="50"/>
       <c r="BM110" s="44"/>
     </row>
-    <row r="111" spans="1:65" x14ac:dyDescent="0.55000000000000004">
+    <row r="111" spans="1:65" x14ac:dyDescent="0.35">
       <c r="A111" s="95"/>
       <c r="B111" s="269" t="s">
         <v>266</v>
@@ -20841,7 +20844,7 @@
       <c r="BL111" s="50"/>
       <c r="BM111" s="44"/>
     </row>
-    <row r="112" spans="1:65" x14ac:dyDescent="0.55000000000000004">
+    <row r="112" spans="1:65" x14ac:dyDescent="0.35">
       <c r="A112" s="95"/>
       <c r="B112" s="269" t="s">
         <v>273</v>
@@ -21028,7 +21031,7 @@
       <c r="BL112" s="50"/>
       <c r="BM112" s="44"/>
     </row>
-    <row r="113" spans="1:65" x14ac:dyDescent="0.55000000000000004">
+    <row r="113" spans="1:65" x14ac:dyDescent="0.35">
       <c r="A113" s="95"/>
       <c r="B113" s="269" t="s">
         <v>299</v>
@@ -21215,7 +21218,7 @@
       <c r="BL113" s="50"/>
       <c r="BM113" s="44"/>
     </row>
-    <row r="114" spans="1:65" x14ac:dyDescent="0.55000000000000004">
+    <row r="114" spans="1:65" x14ac:dyDescent="0.35">
       <c r="A114" s="95"/>
       <c r="B114" s="269" t="s">
         <v>184</v>
@@ -21402,7 +21405,7 @@
       <c r="BL114" s="50"/>
       <c r="BM114" s="44"/>
     </row>
-    <row r="115" spans="1:65" x14ac:dyDescent="0.55000000000000004">
+    <row r="115" spans="1:65" x14ac:dyDescent="0.35">
       <c r="A115" s="95"/>
       <c r="B115" s="443" t="s">
         <v>278</v>
@@ -21589,7 +21592,7 @@
       <c r="BL115" s="50"/>
       <c r="BM115" s="44"/>
     </row>
-    <row r="116" spans="1:65" x14ac:dyDescent="0.55000000000000004">
+    <row r="116" spans="1:65" x14ac:dyDescent="0.35">
       <c r="A116" s="95"/>
       <c r="B116" s="443" t="s">
         <v>279</v>
@@ -21776,7 +21779,7 @@
       <c r="BL116" s="50"/>
       <c r="BM116" s="44"/>
     </row>
-    <row r="117" spans="1:65" x14ac:dyDescent="0.55000000000000004">
+    <row r="117" spans="1:65" x14ac:dyDescent="0.35">
       <c r="A117" s="95"/>
       <c r="B117" s="443" t="s">
         <v>274</v>
@@ -21963,7 +21966,7 @@
       <c r="BL117" s="50"/>
       <c r="BM117" s="44"/>
     </row>
-    <row r="118" spans="1:65" x14ac:dyDescent="0.55000000000000004">
+    <row r="118" spans="1:65" x14ac:dyDescent="0.35">
       <c r="A118" s="95"/>
       <c r="B118" s="444" t="s">
         <v>275</v>
@@ -22150,7 +22153,7 @@
       <c r="BL118" s="50"/>
       <c r="BM118" s="44"/>
     </row>
-    <row r="119" spans="1:65" x14ac:dyDescent="0.55000000000000004">
+    <row r="119" spans="1:65" x14ac:dyDescent="0.35">
       <c r="A119" s="95"/>
       <c r="B119" s="444" t="s">
         <v>276</v>
@@ -22337,7 +22340,7 @@
       <c r="BL119" s="50"/>
       <c r="BM119" s="44"/>
     </row>
-    <row r="120" spans="1:65" x14ac:dyDescent="0.55000000000000004">
+    <row r="120" spans="1:65" x14ac:dyDescent="0.35">
       <c r="A120" s="95"/>
       <c r="B120" s="444" t="s">
         <v>277</v>
@@ -22524,7 +22527,7 @@
       <c r="BL120" s="50"/>
       <c r="BM120" s="44"/>
     </row>
-    <row r="121" spans="1:65" x14ac:dyDescent="0.55000000000000004">
+    <row r="121" spans="1:65" x14ac:dyDescent="0.35">
       <c r="A121" s="95"/>
       <c r="B121" s="444" t="s">
         <v>314</v>
@@ -22711,7 +22714,7 @@
       <c r="BL121" s="50"/>
       <c r="BM121" s="44"/>
     </row>
-    <row r="122" spans="1:65" x14ac:dyDescent="0.55000000000000004">
+    <row r="122" spans="1:65" x14ac:dyDescent="0.35">
       <c r="A122" s="95"/>
       <c r="B122" s="435" t="s">
         <v>287</v>
@@ -22919,7 +22922,7 @@
         <v/>
       </c>
     </row>
-    <row r="123" spans="1:65" x14ac:dyDescent="0.55000000000000004">
+    <row r="123" spans="1:65" x14ac:dyDescent="0.35">
       <c r="A123" s="95"/>
       <c r="B123" s="435" t="s">
         <v>304</v>
@@ -23127,7 +23130,7 @@
         <v/>
       </c>
     </row>
-    <row r="124" spans="1:65" x14ac:dyDescent="0.55000000000000004">
+    <row r="124" spans="1:65" x14ac:dyDescent="0.35">
       <c r="A124" s="95"/>
       <c r="B124" s="435" t="s">
         <v>284</v>
@@ -23335,7 +23338,7 @@
         <v/>
       </c>
     </row>
-    <row r="125" spans="1:65" x14ac:dyDescent="0.55000000000000004">
+    <row r="125" spans="1:65" x14ac:dyDescent="0.35">
       <c r="A125" s="95"/>
       <c r="B125" s="435" t="s">
         <v>302</v>
@@ -23543,7 +23546,7 @@
         <v/>
       </c>
     </row>
-    <row r="126" spans="1:65" x14ac:dyDescent="0.55000000000000004">
+    <row r="126" spans="1:65" x14ac:dyDescent="0.35">
       <c r="A126" s="95"/>
       <c r="B126" s="435" t="s">
         <v>285</v>
@@ -23751,7 +23754,7 @@
         <v/>
       </c>
     </row>
-    <row r="127" spans="1:65" x14ac:dyDescent="0.55000000000000004">
+    <row r="127" spans="1:65" x14ac:dyDescent="0.35">
       <c r="A127" s="95"/>
       <c r="B127" s="435" t="s">
         <v>256</v>
@@ -23959,7 +23962,7 @@
         <v/>
       </c>
     </row>
-    <row r="128" spans="1:65" x14ac:dyDescent="0.55000000000000004">
+    <row r="128" spans="1:65" x14ac:dyDescent="0.35">
       <c r="A128" s="95"/>
       <c r="B128" s="338" t="s">
         <v>185</v>
@@ -24031,7 +24034,7 @@
       <c r="BL128" s="50"/>
       <c r="BM128" s="44"/>
     </row>
-    <row r="129" spans="1:65" s="226" customFormat="1" ht="28.5" x14ac:dyDescent="0.65">
+    <row r="129" spans="1:65" s="226" customFormat="1" ht="28.5" x14ac:dyDescent="0.45">
       <c r="A129" s="310"/>
       <c r="B129" s="327" t="s">
         <v>186</v>
@@ -24100,7 +24103,7 @@
       <c r="BL129" s="214"/>
       <c r="BM129" s="213"/>
     </row>
-    <row r="130" spans="1:65" x14ac:dyDescent="0.55000000000000004">
+    <row r="130" spans="1:65" x14ac:dyDescent="0.35">
       <c r="A130" s="95"/>
       <c r="B130" s="19" t="s">
         <v>300</v>
@@ -24313,7 +24316,7 @@
         <v/>
       </c>
     </row>
-    <row r="131" spans="1:65" x14ac:dyDescent="0.55000000000000004">
+    <row r="131" spans="1:65" x14ac:dyDescent="0.35">
       <c r="A131" s="95"/>
       <c r="B131" s="19" t="s">
         <v>301</v>
@@ -24526,7 +24529,7 @@
         <v/>
       </c>
     </row>
-    <row r="132" spans="1:65" x14ac:dyDescent="0.55000000000000004">
+    <row r="132" spans="1:65" x14ac:dyDescent="0.35">
       <c r="A132" s="95"/>
       <c r="B132" s="19" t="s">
         <v>190</v>
@@ -24718,7 +24721,7 @@
       <c r="BL132" s="50"/>
       <c r="BM132" s="44"/>
     </row>
-    <row r="133" spans="1:65" x14ac:dyDescent="0.55000000000000004">
+    <row r="133" spans="1:65" x14ac:dyDescent="0.35">
       <c r="A133" s="95"/>
       <c r="B133" s="19" t="s">
         <v>191</v>
@@ -24910,7 +24913,7 @@
       <c r="BL133" s="50"/>
       <c r="BM133" s="44"/>
     </row>
-    <row r="134" spans="1:65" x14ac:dyDescent="0.55000000000000004">
+    <row r="134" spans="1:65" x14ac:dyDescent="0.35">
       <c r="A134" s="95"/>
       <c r="B134" s="19" t="s">
         <v>187</v>
@@ -25102,7 +25105,7 @@
       <c r="BL134" s="50"/>
       <c r="BM134" s="44"/>
     </row>
-    <row r="135" spans="1:65" x14ac:dyDescent="0.55000000000000004">
+    <row r="135" spans="1:65" x14ac:dyDescent="0.35">
       <c r="A135" s="95"/>
       <c r="B135" s="19" t="s">
         <v>188</v>
@@ -25294,7 +25297,7 @@
       <c r="BL135" s="50"/>
       <c r="BM135" s="44"/>
     </row>
-    <row r="136" spans="1:65" x14ac:dyDescent="0.55000000000000004">
+    <row r="136" spans="1:65" x14ac:dyDescent="0.35">
       <c r="A136" s="95"/>
       <c r="B136" s="19" t="s">
         <v>189</v>
@@ -25480,7 +25483,7 @@
       <c r="BL136" s="50"/>
       <c r="BM136" s="44"/>
     </row>
-    <row r="137" spans="1:65" x14ac:dyDescent="0.55000000000000004">
+    <row r="137" spans="1:65" x14ac:dyDescent="0.35">
       <c r="A137" s="95"/>
       <c r="B137" s="19" t="s">
         <v>192</v>
@@ -25666,7 +25669,7 @@
       <c r="BL137" s="50"/>
       <c r="BM137" s="44"/>
     </row>
-    <row r="138" spans="1:65" x14ac:dyDescent="0.55000000000000004">
+    <row r="138" spans="1:65" x14ac:dyDescent="0.35">
       <c r="A138" s="95"/>
       <c r="B138" s="19" t="s">
         <v>192</v>
@@ -25852,7 +25855,7 @@
       <c r="BL138" s="50"/>
       <c r="BM138" s="44"/>
     </row>
-    <row r="139" spans="1:65" x14ac:dyDescent="0.55000000000000004">
+    <row r="139" spans="1:65" x14ac:dyDescent="0.35">
       <c r="A139" s="95"/>
       <c r="B139" s="19" t="s">
         <v>193</v>
@@ -26038,7 +26041,7 @@
       <c r="BL139" s="50"/>
       <c r="BM139" s="44"/>
     </row>
-    <row r="140" spans="1:65" hidden="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="140" spans="1:65" hidden="1" x14ac:dyDescent="0.35">
       <c r="A140" s="95"/>
       <c r="B140" s="19" t="s">
         <v>80</v>
@@ -26245,7 +26248,7 @@
         <v/>
       </c>
     </row>
-    <row r="141" spans="1:65" hidden="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="141" spans="1:65" hidden="1" x14ac:dyDescent="0.35">
       <c r="A141" s="95"/>
       <c r="B141" s="19" t="s">
         <v>81</v>
@@ -26452,7 +26455,7 @@
         <v/>
       </c>
     </row>
-    <row r="142" spans="1:65" hidden="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="142" spans="1:65" hidden="1" x14ac:dyDescent="0.35">
       <c r="A142" s="95"/>
       <c r="B142" s="19" t="s">
         <v>82</v>
@@ -26659,7 +26662,7 @@
         <v/>
       </c>
     </row>
-    <row r="143" spans="1:65" hidden="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="143" spans="1:65" hidden="1" x14ac:dyDescent="0.35">
       <c r="A143" s="95"/>
       <c r="B143" s="19" t="s">
         <v>83</v>
@@ -26866,7 +26869,7 @@
         <v/>
       </c>
     </row>
-    <row r="144" spans="1:65" hidden="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="144" spans="1:65" hidden="1" x14ac:dyDescent="0.35">
       <c r="A144" s="95"/>
       <c r="B144" s="19" t="s">
         <v>84</v>
@@ -27073,7 +27076,7 @@
         <v/>
       </c>
     </row>
-    <row r="145" spans="1:65" hidden="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="145" spans="1:65" hidden="1" x14ac:dyDescent="0.35">
       <c r="A145" s="95"/>
       <c r="B145" s="19" t="s">
         <v>85</v>
@@ -27280,7 +27283,7 @@
         <v/>
       </c>
     </row>
-    <row r="146" spans="1:65" ht="24" hidden="1" thickBot="1" x14ac:dyDescent="0.6">
+    <row r="146" spans="1:65" ht="24" hidden="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A146" s="99"/>
       <c r="B146" s="100"/>
       <c r="C146" s="13"/>
@@ -27485,7 +27488,10 @@
         <v/>
       </c>
     </row>
-    <row r="147" spans="1:65" x14ac:dyDescent="0.55000000000000004">
+    <row r="147" spans="1:65" ht="28.5" x14ac:dyDescent="0.45">
+      <c r="B147" s="327" t="s">
+        <v>315</v>
+      </c>
       <c r="V147" s="237" t="str">
         <f>IF($D147&lt;&gt;"",(R147*G147/5),"")</f>
         <v/>
@@ -27497,7 +27503,7 @@
       </c>
       <c r="AG147" s="237"/>
     </row>
-    <row r="148" spans="1:65" x14ac:dyDescent="0.55000000000000004">
+    <row r="148" spans="1:65" x14ac:dyDescent="0.35">
       <c r="A148" s="95"/>
       <c r="B148" s="443" t="s">
         <v>225</v>
@@ -27684,7 +27690,7 @@
       <c r="BL148" s="50"/>
       <c r="BM148" s="44"/>
     </row>
-    <row r="149" spans="1:65" x14ac:dyDescent="0.55000000000000004">
+    <row r="149" spans="1:65" x14ac:dyDescent="0.35">
       <c r="A149" s="95"/>
       <c r="B149" s="443" t="s">
         <v>226</v>
@@ -27871,7 +27877,7 @@
       <c r="BL149" s="50"/>
       <c r="BM149" s="44"/>
     </row>
-    <row r="150" spans="1:65" x14ac:dyDescent="0.55000000000000004">
+    <row r="150" spans="1:65" x14ac:dyDescent="0.35">
       <c r="A150" s="95"/>
       <c r="B150" s="443" t="s">
         <v>227</v>
@@ -28058,7 +28064,7 @@
       <c r="BL150" s="50"/>
       <c r="BM150" s="44"/>
     </row>
-    <row r="151" spans="1:65" x14ac:dyDescent="0.55000000000000004">
+    <row r="151" spans="1:65" x14ac:dyDescent="0.35">
       <c r="A151" s="95"/>
       <c r="B151" s="444" t="s">
         <v>293</v>
@@ -28245,7 +28251,7 @@
       <c r="BL151" s="50"/>
       <c r="BM151" s="44"/>
     </row>
-    <row r="152" spans="1:65" x14ac:dyDescent="0.55000000000000004">
+    <row r="152" spans="1:65" x14ac:dyDescent="0.35">
       <c r="A152" s="95"/>
       <c r="B152" s="444" t="s">
         <v>231</v>
@@ -28432,7 +28438,7 @@
       <c r="BL152" s="50"/>
       <c r="BM152" s="44"/>
     </row>
-    <row r="153" spans="1:65" x14ac:dyDescent="0.55000000000000004">
+    <row r="153" spans="1:65" x14ac:dyDescent="0.35">
       <c r="A153" s="95"/>
       <c r="B153" s="444" t="s">
         <v>240</v>
@@ -28619,7 +28625,7 @@
       <c r="BL153" s="50"/>
       <c r="BM153" s="44"/>
     </row>
-    <row r="154" spans="1:65" ht="23" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="154" spans="1:65" ht="23.1" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B154" s="459" t="s">
         <v>305</v>
       </c>
@@ -28628,7 +28634,7 @@
         <v>NUEVAS RESINAS</v>
       </c>
     </row>
-    <row r="155" spans="1:65" x14ac:dyDescent="0.55000000000000004">
+    <row r="155" spans="1:65" x14ac:dyDescent="0.35">
       <c r="A155" s="95"/>
       <c r="B155" s="455" t="s">
         <v>306</v>
@@ -28814,7 +28820,7 @@
       <c r="BL155" s="50"/>
       <c r="BM155" s="44"/>
     </row>
-    <row r="156" spans="1:65" x14ac:dyDescent="0.55000000000000004">
+    <row r="156" spans="1:65" x14ac:dyDescent="0.35">
       <c r="A156" s="95"/>
       <c r="B156" s="455" t="s">
         <v>307</v>
@@ -29000,7 +29006,7 @@
       <c r="BL156" s="50"/>
       <c r="BM156" s="44"/>
     </row>
-    <row r="157" spans="1:65" x14ac:dyDescent="0.55000000000000004">
+    <row r="157" spans="1:65" x14ac:dyDescent="0.35">
       <c r="A157" s="95"/>
       <c r="B157" s="455" t="s">
         <v>308</v>
@@ -29186,7 +29192,7 @@
       <c r="BL157" s="50"/>
       <c r="BM157" s="44"/>
     </row>
-    <row r="158" spans="1:65" x14ac:dyDescent="0.55000000000000004">
+    <row r="158" spans="1:65" x14ac:dyDescent="0.35">
       <c r="A158" s="95"/>
       <c r="B158" s="455" t="s">
         <v>311</v>
@@ -29372,7 +29378,7 @@
       <c r="BL158" s="50"/>
       <c r="BM158" s="44"/>
     </row>
-    <row r="159" spans="1:65" x14ac:dyDescent="0.55000000000000004">
+    <row r="159" spans="1:65" x14ac:dyDescent="0.35">
       <c r="A159" s="95"/>
       <c r="B159" s="455" t="s">
         <v>312</v>
@@ -29558,7 +29564,7 @@
       <c r="BL159" s="50"/>
       <c r="BM159" s="44"/>
     </row>
-    <row r="160" spans="1:65" x14ac:dyDescent="0.55000000000000004">
+    <row r="160" spans="1:65" x14ac:dyDescent="0.35">
       <c r="A160" s="95"/>
       <c r="B160" s="455" t="s">
         <v>310</v>
@@ -29741,7 +29747,7 @@
       <c r="BL160" s="50"/>
       <c r="BM160" s="44"/>
     </row>
-    <row r="161" spans="1:65" x14ac:dyDescent="0.55000000000000004">
+    <row r="161" spans="1:65" x14ac:dyDescent="0.35">
       <c r="B161" s="460" t="s">
         <v>313</v>
       </c>
@@ -29752,7 +29758,7 @@
         <v>ALTO CONSUMO</v>
       </c>
     </row>
-    <row r="162" spans="1:65" x14ac:dyDescent="0.55000000000000004">
+    <row r="162" spans="1:65" x14ac:dyDescent="0.35">
       <c r="A162" s="95"/>
       <c r="B162" s="455" t="s">
         <v>311</v>
@@ -29938,7 +29944,7 @@
       <c r="BL162" s="50"/>
       <c r="BM162" s="44"/>
     </row>
-    <row r="163" spans="1:65" x14ac:dyDescent="0.55000000000000004">
+    <row r="163" spans="1:65" x14ac:dyDescent="0.35">
       <c r="A163" s="95"/>
       <c r="B163" s="455" t="s">
         <v>312</v>
@@ -30121,7 +30127,7 @@
       <c r="BL163" s="50"/>
       <c r="BM163" s="44"/>
     </row>
-    <row r="164" spans="1:65" x14ac:dyDescent="0.55000000000000004">
+    <row r="164" spans="1:65" x14ac:dyDescent="0.35">
       <c r="A164" s="95"/>
       <c r="B164" s="455" t="s">
         <v>310</v>
@@ -30319,37 +30325,37 @@
       <selection activeCell="B11" sqref="B11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="18.5" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="18.75" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="4" customWidth="1"/>
     <col min="2" max="2" width="58" customWidth="1"/>
-    <col min="3" max="3" width="8.54296875" customWidth="1"/>
-    <col min="4" max="4" width="11.54296875" customWidth="1"/>
-    <col min="5" max="5" width="11.54296875" style="366" customWidth="1"/>
+    <col min="3" max="3" width="8.5703125" customWidth="1"/>
+    <col min="4" max="4" width="11.5703125" customWidth="1"/>
+    <col min="5" max="5" width="11.5703125" style="366" customWidth="1"/>
     <col min="6" max="6" width="19" style="1" customWidth="1"/>
-    <col min="7" max="7" width="5.08984375" customWidth="1"/>
+    <col min="7" max="7" width="5.140625" customWidth="1"/>
     <col min="8" max="8" width="11" style="366" customWidth="1"/>
     <col min="9" max="9" width="17" style="1" customWidth="1"/>
-    <col min="10" max="10" width="4.36328125" customWidth="1"/>
+    <col min="10" max="10" width="4.42578125" customWidth="1"/>
     <col min="11" max="11" width="16" style="366" customWidth="1"/>
-    <col min="12" max="12" width="17.08984375" style="1" customWidth="1"/>
-    <col min="13" max="13" width="4.08984375" customWidth="1"/>
-    <col min="14" max="14" width="14.36328125" style="366" customWidth="1"/>
-    <col min="15" max="15" width="15.90625" style="1" customWidth="1"/>
-    <col min="16" max="16" width="22.90625" customWidth="1"/>
-    <col min="17" max="17" width="5.90625" hidden="1" customWidth="1"/>
-    <col min="18" max="18" width="22.54296875" hidden="1" customWidth="1"/>
+    <col min="12" max="12" width="17.140625" style="1" customWidth="1"/>
+    <col min="13" max="13" width="4.140625" customWidth="1"/>
+    <col min="14" max="14" width="14.42578125" style="366" customWidth="1"/>
+    <col min="15" max="15" width="15.85546875" style="1" customWidth="1"/>
+    <col min="16" max="16" width="22.85546875" customWidth="1"/>
+    <col min="17" max="17" width="5.85546875" hidden="1" customWidth="1"/>
+    <col min="18" max="18" width="22.5703125" hidden="1" customWidth="1"/>
     <col min="19" max="19" width="6" hidden="1" customWidth="1"/>
-    <col min="20" max="20" width="32.36328125" hidden="1" customWidth="1"/>
-    <col min="21" max="21" width="8.453125" hidden="1" customWidth="1"/>
-    <col min="22" max="22" width="7.08984375" hidden="1" customWidth="1"/>
-    <col min="23" max="23" width="8.90625" hidden="1" customWidth="1"/>
-    <col min="24" max="24" width="5.36328125" hidden="1" customWidth="1"/>
-    <col min="25" max="25" width="7.36328125" hidden="1" customWidth="1"/>
+    <col min="20" max="20" width="32.42578125" hidden="1" customWidth="1"/>
+    <col min="21" max="21" width="8.42578125" hidden="1" customWidth="1"/>
+    <col min="22" max="22" width="7.140625" hidden="1" customWidth="1"/>
+    <col min="23" max="23" width="8.85546875" hidden="1" customWidth="1"/>
+    <col min="24" max="24" width="5.42578125" hidden="1" customWidth="1"/>
+    <col min="25" max="25" width="7.42578125" hidden="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:25" ht="103.5" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="2" spans="1:25" s="108" customFormat="1" ht="46" x14ac:dyDescent="1">
+    <row r="1" spans="1:25" ht="103.5" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="2" spans="1:25" s="108" customFormat="1" ht="46.5" x14ac:dyDescent="0.7">
       <c r="B2" s="108" t="s">
         <v>56</v>
       </c>
@@ -30362,7 +30368,7 @@
       <c r="N2" s="366"/>
       <c r="O2" s="1"/>
     </row>
-    <row r="3" spans="1:25" s="108" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="1">
+    <row r="3" spans="1:25" s="108" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.7">
       <c r="A3" s="189"/>
       <c r="B3" s="189"/>
       <c r="C3" s="189"/>
@@ -30389,7 +30395,7 @@
       <c r="X3" s="189"/>
       <c r="Y3" s="189"/>
     </row>
-    <row r="4" spans="1:25" s="189" customFormat="1" ht="19" thickBot="1" x14ac:dyDescent="0.5">
+    <row r="4" spans="1:25" s="189" customFormat="1" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B4" s="193"/>
       <c r="C4" s="194"/>
       <c r="D4" s="194"/>
@@ -30405,7 +30411,7 @@
       <c r="N4" s="366"/>
       <c r="O4" s="1"/>
     </row>
-    <row r="5" spans="1:25" ht="23.5" x14ac:dyDescent="0.55000000000000004">
+    <row r="5" spans="1:25" ht="23.25" x14ac:dyDescent="0.35">
       <c r="A5" s="343"/>
       <c r="B5" s="344"/>
       <c r="C5" s="348"/>
@@ -30438,7 +30444,7 @@
       <c r="X5" s="190"/>
       <c r="Y5" s="190"/>
     </row>
-    <row r="6" spans="1:25" ht="19" thickBot="1" x14ac:dyDescent="0.5">
+    <row r="6" spans="1:25" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A6" s="343"/>
       <c r="B6" s="343"/>
       <c r="C6" s="353" t="s">
@@ -30475,7 +30481,7 @@
         <v>216</v>
       </c>
     </row>
-    <row r="7" spans="1:25" s="1" customFormat="1" x14ac:dyDescent="0.45">
+    <row r="7" spans="1:25" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A7" s="345" t="s">
         <v>0</v>
       </c>
@@ -30532,7 +30538,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="8" spans="1:25" x14ac:dyDescent="0.45">
+    <row r="8" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A8" s="96"/>
       <c r="B8" s="146" t="s">
         <v>219</v>
@@ -30551,7 +30557,7 @@
       <c r="N8" s="382"/>
       <c r="O8" s="69"/>
     </row>
-    <row r="9" spans="1:25" x14ac:dyDescent="0.45">
+    <row r="9" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A9" s="95"/>
       <c r="B9" s="358" t="s">
         <v>224</v>
@@ -30570,7 +30576,7 @@
       <c r="N9" s="383"/>
       <c r="O9" s="16"/>
     </row>
-    <row r="10" spans="1:25" x14ac:dyDescent="0.45">
+    <row r="10" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A10" s="95"/>
       <c r="B10" s="19" t="s">
         <v>225</v>
@@ -30615,7 +30621,7 @@
         <v>356.1</v>
       </c>
     </row>
-    <row r="11" spans="1:25" x14ac:dyDescent="0.45">
+    <row r="11" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A11" s="95"/>
       <c r="B11" s="19" t="s">
         <v>226</v>
@@ -30660,7 +30666,7 @@
         <v>480</v>
       </c>
     </row>
-    <row r="12" spans="1:25" x14ac:dyDescent="0.45">
+    <row r="12" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A12" s="95"/>
       <c r="B12" s="19" t="s">
         <v>227</v>
@@ -30705,7 +30711,7 @@
         <v>354.3</v>
       </c>
     </row>
-    <row r="13" spans="1:25" x14ac:dyDescent="0.45">
+    <row r="13" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A13" s="95"/>
       <c r="B13" s="19" t="s">
         <v>228</v>
@@ -30750,7 +30756,7 @@
         <v>1060.8</v>
       </c>
     </row>
-    <row r="14" spans="1:25" x14ac:dyDescent="0.45">
+    <row r="14" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A14" s="95"/>
       <c r="B14" s="19" t="s">
         <v>229</v>
@@ -30795,7 +30801,7 @@
         <v>581.1</v>
       </c>
     </row>
-    <row r="15" spans="1:25" x14ac:dyDescent="0.45">
+    <row r="15" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A15" s="95"/>
       <c r="B15" s="19" t="s">
         <v>230</v>
@@ -30840,7 +30846,7 @@
         <v>287.40000000000003</v>
       </c>
     </row>
-    <row r="16" spans="1:25" x14ac:dyDescent="0.45">
+    <row r="16" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A16" s="95"/>
       <c r="B16" s="19" t="s">
         <v>231</v>
@@ -30885,7 +30891,7 @@
         <v>266.10000000000002</v>
       </c>
     </row>
-    <row r="17" spans="1:15" x14ac:dyDescent="0.45">
+    <row r="17" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A17" s="95"/>
       <c r="B17" s="19" t="s">
         <v>232</v>
@@ -30930,7 +30936,7 @@
         <v>386.1</v>
       </c>
     </row>
-    <row r="18" spans="1:15" x14ac:dyDescent="0.45">
+    <row r="18" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A18" s="95"/>
       <c r="B18" s="19" t="s">
         <v>240</v>
@@ -30975,7 +30981,7 @@
         <v>353.7</v>
       </c>
     </row>
-    <row r="19" spans="1:15" x14ac:dyDescent="0.45">
+    <row r="19" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A19" s="95"/>
       <c r="B19" s="19"/>
       <c r="C19" s="11"/>
@@ -31016,7 +31022,7 @@
         <v/>
       </c>
     </row>
-    <row r="20" spans="1:15" x14ac:dyDescent="0.45">
+    <row r="20" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A20" s="95"/>
       <c r="B20" s="19"/>
       <c r="C20" s="11"/>
@@ -31057,7 +31063,7 @@
         <v/>
       </c>
     </row>
-    <row r="21" spans="1:15" x14ac:dyDescent="0.45">
+    <row r="21" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A21" s="95"/>
       <c r="B21" s="19"/>
       <c r="C21" s="11"/>
@@ -31098,7 +31104,7 @@
         <v/>
       </c>
     </row>
-    <row r="22" spans="1:15" x14ac:dyDescent="0.45">
+    <row r="22" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A22" s="95"/>
       <c r="B22" s="357" t="s">
         <v>233</v>
@@ -31141,7 +31147,7 @@
         <v/>
       </c>
     </row>
-    <row r="23" spans="1:15" x14ac:dyDescent="0.45">
+    <row r="23" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A23" s="95"/>
       <c r="B23" s="19"/>
       <c r="C23" s="11"/>
@@ -31182,7 +31188,7 @@
         <v/>
       </c>
     </row>
-    <row r="24" spans="1:15" x14ac:dyDescent="0.45">
+    <row r="24" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A24" s="95"/>
       <c r="B24" s="19" t="s">
         <v>234</v>
@@ -31227,7 +31233,7 @@
         <v>990</v>
       </c>
     </row>
-    <row r="25" spans="1:15" x14ac:dyDescent="0.45">
+    <row r="25" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A25" s="95"/>
       <c r="B25" s="19" t="s">
         <v>235</v>
@@ -31272,7 +31278,7 @@
         <v>1200.9000000000001</v>
       </c>
     </row>
-    <row r="26" spans="1:15" x14ac:dyDescent="0.45">
+    <row r="26" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A26" s="95"/>
       <c r="B26" s="19" t="s">
         <v>236</v>
@@ -31317,7 +31323,7 @@
         <v>1320</v>
       </c>
     </row>
-    <row r="27" spans="1:15" x14ac:dyDescent="0.45">
+    <row r="27" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A27" s="95"/>
       <c r="B27" s="19" t="s">
         <v>237</v>
@@ -31362,7 +31368,7 @@
         <v>1275</v>
       </c>
     </row>
-    <row r="28" spans="1:15" x14ac:dyDescent="0.45">
+    <row r="28" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A28" s="95"/>
       <c r="B28" s="19" t="s">
         <v>238</v>
@@ -31407,7 +31413,7 @@
         <v>1006.2</v>
       </c>
     </row>
-    <row r="29" spans="1:15" x14ac:dyDescent="0.45">
+    <row r="29" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A29" s="95"/>
       <c r="B29" s="19" t="s">
         <v>242</v>
@@ -31452,7 +31458,7 @@
         <v>750</v>
       </c>
     </row>
-    <row r="30" spans="1:15" x14ac:dyDescent="0.45">
+    <row r="30" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A30" s="95"/>
       <c r="B30" s="19"/>
       <c r="C30" s="11"/>
@@ -31493,7 +31499,7 @@
         <v/>
       </c>
     </row>
-    <row r="31" spans="1:15" x14ac:dyDescent="0.45">
+    <row r="31" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A31" s="95"/>
       <c r="B31" s="19"/>
       <c r="C31" s="11"/>
@@ -31534,7 +31540,7 @@
         <v/>
       </c>
     </row>
-    <row r="32" spans="1:15" x14ac:dyDescent="0.45">
+    <row r="32" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A32" s="95"/>
       <c r="B32" s="19"/>
       <c r="C32" s="11"/>
@@ -31575,7 +31581,7 @@
         <v/>
       </c>
     </row>
-    <row r="33" spans="1:15" x14ac:dyDescent="0.45">
+    <row r="33" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A33" s="95"/>
       <c r="B33" s="19"/>
       <c r="C33" s="11"/>
@@ -31616,7 +31622,7 @@
         <v/>
       </c>
     </row>
-    <row r="34" spans="1:15" x14ac:dyDescent="0.45">
+    <row r="34" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A34" s="95"/>
       <c r="B34" s="19"/>
       <c r="C34" s="11"/>
@@ -31657,7 +31663,7 @@
         <v/>
       </c>
     </row>
-    <row r="35" spans="1:15" x14ac:dyDescent="0.45">
+    <row r="35" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A35" s="95"/>
       <c r="B35" s="19"/>
       <c r="C35" s="11"/>
@@ -31698,7 +31704,7 @@
         <v/>
       </c>
     </row>
-    <row r="36" spans="1:15" x14ac:dyDescent="0.45">
+    <row r="36" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A36" s="95"/>
       <c r="B36" s="19"/>
       <c r="C36" s="11"/>
@@ -31739,7 +31745,7 @@
         <v/>
       </c>
     </row>
-    <row r="37" spans="1:15" x14ac:dyDescent="0.45">
+    <row r="37" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A37" s="95"/>
       <c r="B37" s="19"/>
       <c r="C37" s="11"/>
@@ -31780,7 +31786,7 @@
         <v/>
       </c>
     </row>
-    <row r="38" spans="1:15" x14ac:dyDescent="0.45">
+    <row r="38" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A38" s="95"/>
       <c r="B38" s="19"/>
       <c r="C38" s="11"/>
@@ -31821,7 +31827,7 @@
         <v/>
       </c>
     </row>
-    <row r="39" spans="1:15" x14ac:dyDescent="0.45">
+    <row r="39" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A39" s="95"/>
       <c r="B39" s="19"/>
       <c r="C39" s="11"/>
@@ -31862,7 +31868,7 @@
         <v/>
       </c>
     </row>
-    <row r="40" spans="1:15" x14ac:dyDescent="0.45">
+    <row r="40" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A40" s="95"/>
       <c r="B40" s="19"/>
       <c r="C40" s="11"/>
@@ -31903,7 +31909,7 @@
         <v/>
       </c>
     </row>
-    <row r="41" spans="1:15" x14ac:dyDescent="0.45">
+    <row r="41" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A41" s="95"/>
       <c r="B41" s="19"/>
       <c r="C41" s="11"/>
@@ -31944,7 +31950,7 @@
         <v/>
       </c>
     </row>
-    <row r="42" spans="1:15" x14ac:dyDescent="0.45">
+    <row r="42" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A42" s="95"/>
       <c r="B42" s="19"/>
       <c r="C42" s="11"/>
@@ -31985,7 +31991,7 @@
         <v/>
       </c>
     </row>
-    <row r="43" spans="1:15" x14ac:dyDescent="0.45">
+    <row r="43" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A43" s="95"/>
       <c r="B43" s="19"/>
       <c r="C43" s="11"/>
@@ -32026,7 +32032,7 @@
         <v/>
       </c>
     </row>
-    <row r="44" spans="1:15" x14ac:dyDescent="0.45">
+    <row r="44" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A44" s="95"/>
       <c r="B44" s="19"/>
       <c r="C44" s="11"/>
@@ -32067,7 +32073,7 @@
         <v/>
       </c>
     </row>
-    <row r="45" spans="1:15" x14ac:dyDescent="0.45">
+    <row r="45" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A45" s="95"/>
       <c r="B45" s="19"/>
       <c r="C45" s="11"/>
@@ -32108,7 +32114,7 @@
         <v/>
       </c>
     </row>
-    <row r="46" spans="1:15" x14ac:dyDescent="0.45">
+    <row r="46" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A46" s="95"/>
       <c r="B46" s="19"/>
       <c r="C46" s="11"/>
@@ -32149,7 +32155,7 @@
         <v/>
       </c>
     </row>
-    <row r="47" spans="1:15" x14ac:dyDescent="0.45">
+    <row r="47" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A47" s="95"/>
       <c r="B47" s="19"/>
       <c r="C47" s="11"/>
@@ -32190,7 +32196,7 @@
         <v/>
       </c>
     </row>
-    <row r="48" spans="1:15" x14ac:dyDescent="0.45">
+    <row r="48" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A48" s="95"/>
       <c r="B48" s="19"/>
       <c r="C48" s="11"/>
@@ -32231,7 +32237,7 @@
         <v/>
       </c>
     </row>
-    <row r="49" spans="1:15" x14ac:dyDescent="0.45">
+    <row r="49" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A49" s="95"/>
       <c r="B49" s="19"/>
       <c r="C49" s="11"/>
@@ -32272,7 +32278,7 @@
         <v/>
       </c>
     </row>
-    <row r="50" spans="1:15" x14ac:dyDescent="0.45">
+    <row r="50" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A50" s="95"/>
       <c r="B50" s="19"/>
       <c r="C50" s="11"/>
@@ -32313,7 +32319,7 @@
         <v/>
       </c>
     </row>
-    <row r="51" spans="1:15" x14ac:dyDescent="0.45">
+    <row r="51" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A51" s="95"/>
       <c r="B51" s="19"/>
       <c r="C51" s="11"/>
@@ -32354,7 +32360,7 @@
         <v/>
       </c>
     </row>
-    <row r="52" spans="1:15" x14ac:dyDescent="0.45">
+    <row r="52" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A52" s="95"/>
       <c r="B52" s="19"/>
       <c r="C52" s="11"/>
@@ -32395,7 +32401,7 @@
         <v/>
       </c>
     </row>
-    <row r="53" spans="1:15" x14ac:dyDescent="0.45">
+    <row r="53" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A53" s="95"/>
       <c r="B53" s="19"/>
       <c r="C53" s="11"/>
@@ -32451,58 +32457,58 @@
       <selection activeCell="AM40" sqref="AM40"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="4" customWidth="1"/>
     <col min="2" max="2" width="58" customWidth="1"/>
-    <col min="3" max="3" width="16.453125" customWidth="1"/>
+    <col min="3" max="3" width="16.42578125" customWidth="1"/>
     <col min="4" max="4" width="15" customWidth="1"/>
-    <col min="5" max="5" width="12.08984375" customWidth="1"/>
-    <col min="6" max="6" width="17.453125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="9.90625" customWidth="1"/>
-    <col min="8" max="8" width="13.36328125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="12.140625" customWidth="1"/>
+    <col min="6" max="6" width="17.42578125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="9.85546875" customWidth="1"/>
+    <col min="8" max="8" width="13.42578125" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="5" customWidth="1"/>
-    <col min="10" max="10" width="16.36328125" hidden="1" customWidth="1"/>
-    <col min="11" max="11" width="15.6328125" hidden="1" customWidth="1"/>
-    <col min="12" max="12" width="8.453125" hidden="1" customWidth="1"/>
-    <col min="13" max="13" width="19.453125" hidden="1" customWidth="1"/>
-    <col min="14" max="14" width="8.08984375" hidden="1" customWidth="1"/>
-    <col min="15" max="15" width="9.453125" hidden="1" customWidth="1"/>
+    <col min="10" max="10" width="16.42578125" hidden="1" customWidth="1"/>
+    <col min="11" max="11" width="15.5703125" hidden="1" customWidth="1"/>
+    <col min="12" max="12" width="8.42578125" hidden="1" customWidth="1"/>
+    <col min="13" max="13" width="19.42578125" hidden="1" customWidth="1"/>
+    <col min="14" max="14" width="8.140625" hidden="1" customWidth="1"/>
+    <col min="15" max="15" width="9.42578125" hidden="1" customWidth="1"/>
     <col min="16" max="16" width="8" customWidth="1"/>
     <col min="17" max="17" width="5" customWidth="1"/>
-    <col min="18" max="18" width="15.54296875" hidden="1" customWidth="1"/>
-    <col min="19" max="19" width="12.36328125" hidden="1" customWidth="1"/>
-    <col min="20" max="20" width="8.6328125" hidden="1" customWidth="1"/>
-    <col min="21" max="21" width="23.6328125" hidden="1" customWidth="1"/>
-    <col min="22" max="22" width="7.6328125" hidden="1" customWidth="1"/>
-    <col min="23" max="23" width="8.90625" hidden="1" customWidth="1"/>
-    <col min="24" max="24" width="8.90625" customWidth="1"/>
-    <col min="25" max="25" width="2.36328125" customWidth="1"/>
-    <col min="26" max="26" width="41.6328125" style="200" customWidth="1"/>
-    <col min="27" max="27" width="5.6328125" customWidth="1"/>
+    <col min="18" max="18" width="15.5703125" hidden="1" customWidth="1"/>
+    <col min="19" max="19" width="12.42578125" hidden="1" customWidth="1"/>
+    <col min="20" max="20" width="8.5703125" hidden="1" customWidth="1"/>
+    <col min="21" max="21" width="23.5703125" hidden="1" customWidth="1"/>
+    <col min="22" max="22" width="7.5703125" hidden="1" customWidth="1"/>
+    <col min="23" max="23" width="8.85546875" hidden="1" customWidth="1"/>
+    <col min="24" max="24" width="8.85546875" customWidth="1"/>
+    <col min="25" max="25" width="2.42578125" customWidth="1"/>
+    <col min="26" max="26" width="41.5703125" style="200" customWidth="1"/>
+    <col min="27" max="27" width="5.5703125" customWidth="1"/>
     <col min="28" max="29" width="1" customWidth="1"/>
-    <col min="30" max="30" width="0.453125" customWidth="1"/>
-    <col min="31" max="31" width="18.6328125" customWidth="1"/>
-    <col min="32" max="32" width="9.453125" customWidth="1"/>
-    <col min="33" max="33" width="10.453125" customWidth="1"/>
-    <col min="34" max="34" width="7.6328125" customWidth="1"/>
-    <col min="35" max="35" width="2.36328125" customWidth="1"/>
-    <col min="36" max="36" width="0.90625" customWidth="1"/>
+    <col min="30" max="30" width="0.42578125" customWidth="1"/>
+    <col min="31" max="31" width="18.5703125" customWidth="1"/>
+    <col min="32" max="32" width="9.42578125" customWidth="1"/>
+    <col min="33" max="33" width="10.42578125" customWidth="1"/>
+    <col min="34" max="34" width="7.5703125" customWidth="1"/>
+    <col min="35" max="35" width="2.42578125" customWidth="1"/>
+    <col min="36" max="36" width="0.85546875" customWidth="1"/>
     <col min="37" max="37" width="1" customWidth="1"/>
-    <col min="38" max="38" width="0.6328125" customWidth="1"/>
-    <col min="39" max="39" width="19.08984375" customWidth="1"/>
-    <col min="40" max="40" width="8.08984375" customWidth="1"/>
-    <col min="41" max="42" width="8.54296875" customWidth="1"/>
+    <col min="38" max="38" width="0.5703125" customWidth="1"/>
+    <col min="39" max="39" width="19.140625" customWidth="1"/>
+    <col min="40" max="40" width="8.140625" customWidth="1"/>
+    <col min="41" max="42" width="8.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:42" ht="103.5" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="2" spans="1:42" s="108" customFormat="1" ht="46" x14ac:dyDescent="1">
+    <row r="1" spans="1:42" ht="103.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="2" spans="1:42" s="108" customFormat="1" ht="46.5" x14ac:dyDescent="0.7">
       <c r="B2" s="108" t="s">
         <v>56</v>
       </c>
       <c r="Z2" s="201"/>
     </row>
-    <row r="3" spans="1:42" s="108" customFormat="1" ht="17.25" hidden="1" customHeight="1" x14ac:dyDescent="1">
+    <row r="3" spans="1:42" s="108" customFormat="1" ht="17.25" hidden="1" customHeight="1" x14ac:dyDescent="0.7">
       <c r="A3" s="189"/>
       <c r="B3" s="189"/>
       <c r="C3" s="189"/>
@@ -32546,7 +32552,7 @@
       <c r="AO3" s="189"/>
       <c r="AP3" s="189"/>
     </row>
-    <row r="4" spans="1:42" s="189" customFormat="1" ht="15.5" hidden="1" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:42" s="189" customFormat="1" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
       <c r="B4" s="190" t="s">
         <v>57</v>
       </c>
@@ -32563,7 +32569,7 @@
       <c r="O4" s="195"/>
       <c r="Z4" s="202"/>
     </row>
-    <row r="5" spans="1:42" s="189" customFormat="1" ht="15.5" hidden="1" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:42" s="189" customFormat="1" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
       <c r="B5" s="192" t="s">
         <v>58</v>
       </c>
@@ -32590,7 +32596,7 @@
       <c r="O5" s="197"/>
       <c r="Z5" s="202"/>
     </row>
-    <row r="6" spans="1:42" s="189" customFormat="1" ht="15.5" hidden="1" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:42" s="189" customFormat="1" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
       <c r="B6" s="192" t="s">
         <v>59</v>
       </c>
@@ -32617,7 +32623,7 @@
       <c r="O6" s="197"/>
       <c r="Z6" s="202"/>
     </row>
-    <row r="7" spans="1:42" s="189" customFormat="1" ht="15.5" hidden="1" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:42" s="189" customFormat="1" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
       <c r="B7" s="193"/>
       <c r="C7" s="194"/>
       <c r="D7" s="194"/>
@@ -32632,7 +32638,7 @@
       <c r="O7" s="194"/>
       <c r="Z7" s="202"/>
     </row>
-    <row r="8" spans="1:42" s="189" customFormat="1" ht="15.5" hidden="1" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:42" s="189" customFormat="1" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
       <c r="B8" s="190" t="s">
         <v>66</v>
       </c>
@@ -32649,7 +32655,7 @@
       <c r="O8" s="194"/>
       <c r="Z8" s="202"/>
     </row>
-    <row r="9" spans="1:42" s="189" customFormat="1" ht="15.5" hidden="1" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:42" s="189" customFormat="1" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
       <c r="B9" s="192" t="s">
         <v>58</v>
       </c>
@@ -32676,7 +32682,7 @@
       <c r="O9" s="194"/>
       <c r="Z9" s="202"/>
     </row>
-    <row r="10" spans="1:42" s="189" customFormat="1" ht="15.5" hidden="1" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:42" s="189" customFormat="1" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
       <c r="B10" s="192" t="s">
         <v>64</v>
       </c>
@@ -32703,7 +32709,7 @@
       <c r="O10" s="194"/>
       <c r="Z10" s="202"/>
     </row>
-    <row r="11" spans="1:42" s="189" customFormat="1" ht="16" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="11" spans="1:42" s="189" customFormat="1" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B11" s="193"/>
       <c r="C11" s="194"/>
       <c r="D11" s="194"/>
@@ -32712,7 +32718,7 @@
       <c r="G11" s="194"/>
       <c r="Z11" s="202"/>
     </row>
-    <row r="12" spans="1:42" ht="24" thickBot="1" x14ac:dyDescent="0.6">
+    <row r="12" spans="1:42" ht="24" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A12" s="90"/>
       <c r="B12" s="25" t="s">
         <v>50</v>
@@ -32768,7 +32774,7 @@
       <c r="AO12" s="175"/>
       <c r="AP12" s="176"/>
     </row>
-    <row r="13" spans="1:42" ht="16" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="13" spans="1:42" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A13" s="91"/>
       <c r="B13" s="40"/>
       <c r="C13" s="92" t="s">
@@ -32836,7 +32842,7 @@
       <c r="AO13" s="153"/>
       <c r="AP13" s="155"/>
     </row>
-    <row r="14" spans="1:42" s="1" customFormat="1" ht="21.5" thickBot="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="14" spans="1:42" s="1" customFormat="1" ht="21.75" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A14" s="94" t="s">
         <v>0</v>
       </c>
@@ -32954,7 +32960,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="15" spans="1:42" s="1" customFormat="1" ht="18.5" x14ac:dyDescent="0.45">
+    <row r="15" spans="1:42" s="1" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A15" s="4"/>
       <c r="B15" s="18"/>
       <c r="C15" s="8"/>
@@ -33001,7 +33007,7 @@
       <c r="AO15" s="5"/>
       <c r="AP15" s="9"/>
     </row>
-    <row r="16" spans="1:42" ht="18.5" x14ac:dyDescent="0.45">
+    <row r="16" spans="1:42" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A16" s="95"/>
       <c r="B16" s="19"/>
       <c r="C16" s="11"/>
@@ -33141,7 +33147,7 @@
         <v/>
       </c>
     </row>
-    <row r="17" spans="1:42" ht="18.5" x14ac:dyDescent="0.45">
+    <row r="17" spans="1:42" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A17" s="96"/>
       <c r="B17" s="146" t="s">
         <v>208</v>
@@ -33190,7 +33196,7 @@
       <c r="AO17" s="73"/>
       <c r="AP17" s="71"/>
     </row>
-    <row r="18" spans="1:42" ht="18.5" x14ac:dyDescent="0.45">
+    <row r="18" spans="1:42" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A18" s="95"/>
       <c r="B18" s="19"/>
       <c r="C18" s="11"/>
@@ -33327,7 +33333,7 @@
         <v/>
       </c>
     </row>
-    <row r="19" spans="1:42" ht="18.5" x14ac:dyDescent="0.45">
+    <row r="19" spans="1:42" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A19" s="95"/>
       <c r="B19" s="19"/>
       <c r="C19" s="11"/>
@@ -33464,7 +33470,7 @@
         <v/>
       </c>
     </row>
-    <row r="20" spans="1:42" ht="18.5" x14ac:dyDescent="0.45">
+    <row r="20" spans="1:42" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A20" s="95"/>
       <c r="B20" s="2" t="s">
         <v>123</v>
@@ -33612,7 +33618,7 @@
         <v>15.926400000000001</v>
       </c>
     </row>
-    <row r="21" spans="1:42" ht="18.5" x14ac:dyDescent="0.45">
+    <row r="21" spans="1:42" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A21" s="95"/>
       <c r="B21" s="2" t="s">
         <v>119</v>
@@ -33751,7 +33757,7 @@
         <v/>
       </c>
     </row>
-    <row r="22" spans="1:42" ht="18.5" x14ac:dyDescent="0.45">
+    <row r="22" spans="1:42" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A22" s="95"/>
       <c r="B22" s="2" t="s">
         <v>120</v>
@@ -33899,7 +33905,7 @@
         <v>17.24832</v>
       </c>
     </row>
-    <row r="23" spans="1:42" ht="18.5" x14ac:dyDescent="0.45">
+    <row r="23" spans="1:42" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A23" s="95"/>
       <c r="B23" s="2" t="s">
         <v>119</v>
@@ -34038,7 +34044,7 @@
         <v/>
       </c>
     </row>
-    <row r="24" spans="1:42" ht="18.5" x14ac:dyDescent="0.45">
+    <row r="24" spans="1:42" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A24" s="95"/>
       <c r="B24" s="2" t="s">
         <v>121</v>
@@ -34186,7 +34192,7 @@
         <v>23.792340000000006</v>
       </c>
     </row>
-    <row r="25" spans="1:42" ht="18.5" x14ac:dyDescent="0.45">
+    <row r="25" spans="1:42" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A25" s="95"/>
       <c r="B25" s="2" t="s">
         <v>119</v>
@@ -34325,7 +34331,7 @@
         <v/>
       </c>
     </row>
-    <row r="26" spans="1:42" ht="18.5" x14ac:dyDescent="0.45">
+    <row r="26" spans="1:42" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A26" s="95"/>
       <c r="B26" s="2" t="s">
         <v>122</v>
@@ -34473,7 +34479,7 @@
         <v>13.377000000000001</v>
       </c>
     </row>
-    <row r="27" spans="1:42" ht="18.5" x14ac:dyDescent="0.45">
+    <row r="27" spans="1:42" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A27" s="95"/>
       <c r="B27" s="2" t="s">
         <v>119</v>
@@ -34612,7 +34618,7 @@
         <v/>
       </c>
     </row>
-    <row r="28" spans="1:42" ht="18.5" x14ac:dyDescent="0.45">
+    <row r="28" spans="1:42" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A28" s="95"/>
       <c r="B28" s="2" t="s">
         <v>130</v>
@@ -34760,7 +34766,7 @@
         <v>17.751899999999999</v>
       </c>
     </row>
-    <row r="29" spans="1:42" ht="18.5" x14ac:dyDescent="0.45">
+    <row r="29" spans="1:42" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A29" s="95"/>
       <c r="B29" s="2" t="s">
         <v>119</v>
@@ -34899,7 +34905,7 @@
         <v/>
       </c>
     </row>
-    <row r="30" spans="1:42" ht="18.5" x14ac:dyDescent="0.45">
+    <row r="30" spans="1:42" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A30" s="95"/>
       <c r="B30" s="2" t="s">
         <v>139</v>
@@ -35047,7 +35053,7 @@
         <v>17.320440000000001</v>
       </c>
     </row>
-    <row r="31" spans="1:42" ht="18.5" x14ac:dyDescent="0.45">
+    <row r="31" spans="1:42" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A31" s="95"/>
       <c r="B31" s="2" t="s">
         <v>140</v>
@@ -35195,7 +35201,7 @@
         <v>20.34066</v>
       </c>
     </row>
-    <row r="32" spans="1:42" ht="18.5" x14ac:dyDescent="0.45">
+    <row r="32" spans="1:42" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A32" s="95"/>
       <c r="B32" s="2" t="s">
         <v>143</v>
@@ -35343,7 +35349,7 @@
         <v>25.518179999999997</v>
       </c>
     </row>
-    <row r="33" spans="1:42" ht="18.5" x14ac:dyDescent="0.45">
+    <row r="33" spans="1:42" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A33" s="95"/>
       <c r="B33" s="2" t="s">
         <v>141</v>
@@ -35491,7 +35497,7 @@
         <v>17.751899999999999</v>
       </c>
     </row>
-    <row r="34" spans="1:42" ht="18.5" x14ac:dyDescent="0.45">
+    <row r="34" spans="1:42" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A34" s="95"/>
       <c r="B34" s="2" t="s">
         <v>142</v>
@@ -35639,7 +35645,7 @@
         <v>18.18336</v>
       </c>
     </row>
-    <row r="35" spans="1:42" ht="18.5" x14ac:dyDescent="0.45">
+    <row r="35" spans="1:42" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A35" s="95"/>
       <c r="B35" s="19"/>
       <c r="C35" s="11"/>
@@ -35683,7 +35689,7 @@
       <c r="AO35" s="44"/>
       <c r="AP35" s="42"/>
     </row>
-    <row r="36" spans="1:42" ht="18.5" x14ac:dyDescent="0.45">
+    <row r="36" spans="1:42" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A36" s="95"/>
       <c r="B36" s="19"/>
       <c r="C36" s="11"/>
@@ -35727,7 +35733,7 @@
       <c r="AO36" s="44"/>
       <c r="AP36" s="42"/>
     </row>
-    <row r="37" spans="1:42" ht="18.5" x14ac:dyDescent="0.45">
+    <row r="37" spans="1:42" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A37" s="95"/>
       <c r="B37" s="19"/>
       <c r="C37" s="11"/>
@@ -35771,7 +35777,7 @@
       <c r="AO37" s="44"/>
       <c r="AP37" s="42"/>
     </row>
-    <row r="38" spans="1:42" ht="18.5" x14ac:dyDescent="0.45">
+    <row r="38" spans="1:42" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A38" s="95"/>
       <c r="B38" s="2" t="s">
         <v>134</v>
@@ -35919,7 +35925,7 @@
         <v>17.409600000000001</v>
       </c>
     </row>
-    <row r="39" spans="1:42" ht="18.5" x14ac:dyDescent="0.45">
+    <row r="39" spans="1:42" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A39" s="95"/>
       <c r="B39" s="2" t="s">
         <v>119</v>
@@ -36061,7 +36067,7 @@
         <v/>
       </c>
     </row>
-    <row r="40" spans="1:42" ht="18.5" x14ac:dyDescent="0.45">
+    <row r="40" spans="1:42" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A40" s="95"/>
       <c r="B40" s="2" t="s">
         <v>135</v>
@@ -36209,7 +36215,7 @@
         <v>18.235800000000001</v>
       </c>
     </row>
-    <row r="41" spans="1:42" ht="18.5" x14ac:dyDescent="0.45">
+    <row r="41" spans="1:42" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A41" s="95"/>
       <c r="B41" s="2" t="s">
         <v>119</v>
@@ -36351,7 +36357,7 @@
         <v/>
       </c>
     </row>
-    <row r="42" spans="1:42" ht="18.5" x14ac:dyDescent="0.45">
+    <row r="42" spans="1:42" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A42" s="95"/>
       <c r="B42" s="2" t="s">
         <v>136</v>
@@ -36499,7 +36505,7 @@
         <v>24.845400000000001</v>
       </c>
     </row>
-    <row r="43" spans="1:42" ht="18.5" x14ac:dyDescent="0.45">
+    <row r="43" spans="1:42" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A43" s="95"/>
       <c r="B43" s="2" t="s">
         <v>119</v>
@@ -36641,7 +36647,7 @@
         <v/>
       </c>
     </row>
-    <row r="44" spans="1:42" ht="18.5" x14ac:dyDescent="0.45">
+    <row r="44" spans="1:42" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A44" s="95"/>
       <c r="B44" s="2" t="s">
         <v>144</v>
@@ -36789,7 +36795,7 @@
         <v>26.497799999999998</v>
       </c>
     </row>
-    <row r="45" spans="1:42" ht="18.5" x14ac:dyDescent="0.45">
+    <row r="45" spans="1:42" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A45" s="95"/>
       <c r="B45" s="271" t="s">
         <v>145</v>
@@ -36931,7 +36937,7 @@
         <v/>
       </c>
     </row>
-    <row r="46" spans="1:42" ht="18.5" x14ac:dyDescent="0.45">
+    <row r="46" spans="1:42" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A46" s="95"/>
       <c r="B46" s="2" t="s">
         <v>137</v>
@@ -37079,7 +37085,7 @@
         <v>14.104800000000001</v>
       </c>
     </row>
-    <row r="47" spans="1:42" ht="18.5" x14ac:dyDescent="0.45">
+    <row r="47" spans="1:42" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A47" s="95"/>
       <c r="B47" s="2" t="s">
         <v>119</v>
@@ -37221,7 +37227,7 @@
         <v/>
       </c>
     </row>
-    <row r="48" spans="1:42" ht="18.5" x14ac:dyDescent="0.45">
+    <row r="48" spans="1:42" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A48" s="95"/>
       <c r="B48" s="19"/>
       <c r="C48" s="11"/>
@@ -37265,7 +37271,7 @@
       <c r="AO48" s="44"/>
       <c r="AP48" s="42"/>
     </row>
-    <row r="49" spans="1:42" ht="18.5" x14ac:dyDescent="0.45">
+    <row r="49" spans="1:42" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A49" s="95"/>
       <c r="B49" s="19" t="s">
         <v>138</v>
@@ -37413,7 +37419,7 @@
         <v>87.223500000000016</v>
       </c>
     </row>
-    <row r="50" spans="1:42" ht="18.5" x14ac:dyDescent="0.45">
+    <row r="50" spans="1:42" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A50" s="95"/>
       <c r="B50" s="19"/>
       <c r="C50" s="11"/>
@@ -37553,7 +37559,7 @@
         <v/>
       </c>
     </row>
-    <row r="51" spans="1:42" ht="18.5" x14ac:dyDescent="0.45">
+    <row r="51" spans="1:42" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A51" s="97"/>
       <c r="B51" s="147" t="s">
         <v>10</v>
@@ -37611,7 +37617,7 @@
       <c r="AO51" s="86"/>
       <c r="AP51" s="84"/>
     </row>
-    <row r="52" spans="1:42" ht="18.5" x14ac:dyDescent="0.45">
+    <row r="52" spans="1:42" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A52" s="95"/>
       <c r="B52" s="19" t="s">
         <v>16</v>
@@ -37759,7 +37765,7 @@
         <v>37.078200000000002</v>
       </c>
     </row>
-    <row r="53" spans="1:42" ht="18.5" x14ac:dyDescent="0.45">
+    <row r="53" spans="1:42" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A53" s="95"/>
       <c r="B53" s="19" t="s">
         <v>17</v>
@@ -37907,7 +37913,7 @@
         <v>15.866999999999999</v>
       </c>
     </row>
-    <row r="54" spans="1:42" ht="18.5" x14ac:dyDescent="0.45">
+    <row r="54" spans="1:42" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A54" s="95"/>
       <c r="B54" s="19" t="s">
         <v>18</v>
@@ -38055,7 +38061,7 @@
         <v>45.070200000000007</v>
       </c>
     </row>
-    <row r="55" spans="1:42" ht="18.5" x14ac:dyDescent="0.45">
+    <row r="55" spans="1:42" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A55" s="95"/>
       <c r="B55" s="19"/>
       <c r="C55" s="11"/>
@@ -38195,7 +38201,7 @@
         <v/>
       </c>
     </row>
-    <row r="56" spans="1:42" ht="18.5" x14ac:dyDescent="0.45">
+    <row r="56" spans="1:42" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A56" s="95"/>
       <c r="B56" s="19"/>
       <c r="C56" s="11"/>
@@ -38335,7 +38341,7 @@
         <v/>
       </c>
     </row>
-    <row r="57" spans="1:42" ht="18.5" x14ac:dyDescent="0.45">
+    <row r="57" spans="1:42" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A57" s="95"/>
       <c r="B57" s="19"/>
       <c r="C57" s="11"/>
@@ -38475,7 +38481,7 @@
         <v/>
       </c>
     </row>
-    <row r="58" spans="1:42" ht="18.5" x14ac:dyDescent="0.45">
+    <row r="58" spans="1:42" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A58" s="95"/>
       <c r="B58" s="19"/>
       <c r="C58" s="11"/>
@@ -38615,7 +38621,7 @@
         <v/>
       </c>
     </row>
-    <row r="59" spans="1:42" ht="18.5" x14ac:dyDescent="0.45">
+    <row r="59" spans="1:42" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A59" s="98"/>
       <c r="B59" s="3" t="s">
         <v>20</v>
@@ -38673,7 +38679,7 @@
       <c r="AO59" s="61"/>
       <c r="AP59" s="204"/>
     </row>
-    <row r="60" spans="1:42" ht="18.5" x14ac:dyDescent="0.45">
+    <row r="60" spans="1:42" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A60" s="95"/>
       <c r="B60" s="19" t="s">
         <v>21</v>
@@ -38821,7 +38827,7 @@
         <v>12.3</v>
       </c>
     </row>
-    <row r="61" spans="1:42" ht="18.5" x14ac:dyDescent="0.45">
+    <row r="61" spans="1:42" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A61" s="95"/>
       <c r="B61" s="19" t="s">
         <v>22</v>
@@ -38965,7 +38971,7 @@
         <v/>
       </c>
     </row>
-    <row r="62" spans="1:42" ht="18.5" x14ac:dyDescent="0.45">
+    <row r="62" spans="1:42" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A62" s="95"/>
       <c r="B62" s="19"/>
       <c r="C62" s="11"/>
@@ -39105,7 +39111,7 @@
         <v/>
       </c>
     </row>
-    <row r="63" spans="1:42" ht="18.5" x14ac:dyDescent="0.45">
+    <row r="63" spans="1:42" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A63" s="95"/>
       <c r="B63" s="19" t="s">
         <v>23</v>
@@ -39253,7 +39259,7 @@
         <v>13.020000000000001</v>
       </c>
     </row>
-    <row r="64" spans="1:42" ht="19" thickBot="1" x14ac:dyDescent="0.5">
+    <row r="64" spans="1:42" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A64" s="99"/>
       <c r="B64" s="100"/>
       <c r="C64" s="13"/>
@@ -39405,57 +39411,57 @@
       <selection activeCell="A24" sqref="A24:XFD24"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="4" customWidth="1"/>
     <col min="2" max="2" width="58" customWidth="1"/>
-    <col min="3" max="3" width="16.453125" customWidth="1"/>
+    <col min="3" max="3" width="16.42578125" customWidth="1"/>
     <col min="4" max="4" width="15" customWidth="1"/>
-    <col min="5" max="5" width="12.08984375" customWidth="1"/>
-    <col min="6" max="6" width="17.453125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="9.90625" customWidth="1"/>
-    <col min="8" max="8" width="13.36328125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="12.140625" customWidth="1"/>
+    <col min="6" max="6" width="17.42578125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="9.85546875" customWidth="1"/>
+    <col min="8" max="8" width="13.42578125" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="5" customWidth="1"/>
-    <col min="10" max="10" width="16.36328125" customWidth="1"/>
-    <col min="11" max="11" width="15.6328125" customWidth="1"/>
-    <col min="12" max="12" width="8.453125" customWidth="1"/>
-    <col min="13" max="13" width="19.453125" customWidth="1"/>
-    <col min="14" max="14" width="8.08984375" customWidth="1"/>
-    <col min="15" max="15" width="9.453125" customWidth="1"/>
+    <col min="10" max="10" width="16.42578125" customWidth="1"/>
+    <col min="11" max="11" width="15.5703125" customWidth="1"/>
+    <col min="12" max="12" width="8.42578125" customWidth="1"/>
+    <col min="13" max="13" width="19.42578125" customWidth="1"/>
+    <col min="14" max="14" width="8.140625" customWidth="1"/>
+    <col min="15" max="15" width="9.42578125" customWidth="1"/>
     <col min="16" max="16" width="8" customWidth="1"/>
     <col min="17" max="17" width="5" customWidth="1"/>
-    <col min="18" max="18" width="15.54296875" customWidth="1"/>
-    <col min="19" max="19" width="12.36328125" customWidth="1"/>
-    <col min="20" max="20" width="8.6328125" customWidth="1"/>
-    <col min="21" max="21" width="23.6328125" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="7.6328125" customWidth="1"/>
-    <col min="23" max="24" width="8.90625" customWidth="1"/>
-    <col min="25" max="25" width="2.36328125" customWidth="1"/>
-    <col min="26" max="26" width="41.6328125" style="200" customWidth="1"/>
-    <col min="27" max="27" width="5.6328125" customWidth="1"/>
+    <col min="18" max="18" width="15.5703125" customWidth="1"/>
+    <col min="19" max="19" width="12.42578125" customWidth="1"/>
+    <col min="20" max="20" width="8.5703125" customWidth="1"/>
+    <col min="21" max="21" width="23.5703125" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="7.5703125" customWidth="1"/>
+    <col min="23" max="24" width="8.85546875" customWidth="1"/>
+    <col min="25" max="25" width="2.42578125" customWidth="1"/>
+    <col min="26" max="26" width="41.5703125" style="200" customWidth="1"/>
+    <col min="27" max="27" width="5.5703125" customWidth="1"/>
     <col min="28" max="29" width="1" customWidth="1"/>
-    <col min="30" max="30" width="0.453125" customWidth="1"/>
-    <col min="31" max="31" width="18.6328125" customWidth="1"/>
-    <col min="32" max="32" width="9.453125" customWidth="1"/>
-    <col min="33" max="33" width="10.453125" customWidth="1"/>
-    <col min="34" max="34" width="7.6328125" customWidth="1"/>
-    <col min="35" max="35" width="2.36328125" customWidth="1"/>
-    <col min="36" max="36" width="0.90625" customWidth="1"/>
+    <col min="30" max="30" width="0.42578125" customWidth="1"/>
+    <col min="31" max="31" width="18.5703125" customWidth="1"/>
+    <col min="32" max="32" width="9.42578125" customWidth="1"/>
+    <col min="33" max="33" width="10.42578125" customWidth="1"/>
+    <col min="34" max="34" width="7.5703125" customWidth="1"/>
+    <col min="35" max="35" width="2.42578125" customWidth="1"/>
+    <col min="36" max="36" width="0.85546875" customWidth="1"/>
     <col min="37" max="37" width="1" customWidth="1"/>
-    <col min="38" max="38" width="0.6328125" customWidth="1"/>
-    <col min="39" max="39" width="19.08984375" customWidth="1"/>
-    <col min="40" max="40" width="8.08984375" customWidth="1"/>
-    <col min="41" max="42" width="8.54296875" customWidth="1"/>
+    <col min="38" max="38" width="0.5703125" customWidth="1"/>
+    <col min="39" max="39" width="19.140625" customWidth="1"/>
+    <col min="40" max="40" width="8.140625" customWidth="1"/>
+    <col min="41" max="42" width="8.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:42" ht="103.5" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="2" spans="1:42" s="108" customFormat="1" ht="46" x14ac:dyDescent="1">
+    <row r="1" spans="1:42" ht="103.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="2" spans="1:42" s="108" customFormat="1" ht="46.5" x14ac:dyDescent="0.7">
       <c r="B2" s="108" t="s">
         <v>56</v>
       </c>
       <c r="Z2" s="201"/>
     </row>
-    <row r="3" spans="1:42" s="108" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="1">
+    <row r="3" spans="1:42" s="108" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.7">
       <c r="A3" s="189"/>
       <c r="B3" s="189"/>
       <c r="C3" s="189"/>
@@ -39499,7 +39505,7 @@
       <c r="AO3" s="189"/>
       <c r="AP3" s="189"/>
     </row>
-    <row r="4" spans="1:42" s="189" customFormat="1" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:42" s="189" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B4" s="190" t="s">
         <v>57</v>
       </c>
@@ -39516,7 +39522,7 @@
       <c r="O4" s="195"/>
       <c r="Z4" s="202"/>
     </row>
-    <row r="5" spans="1:42" s="189" customFormat="1" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:42" s="189" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B5" s="192" t="s">
         <v>58</v>
       </c>
@@ -39543,7 +39549,7 @@
       <c r="O5" s="197"/>
       <c r="Z5" s="202"/>
     </row>
-    <row r="6" spans="1:42" s="189" customFormat="1" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:42" s="189" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B6" s="192" t="s">
         <v>59</v>
       </c>
@@ -39570,7 +39576,7 @@
       <c r="O6" s="197"/>
       <c r="Z6" s="202"/>
     </row>
-    <row r="7" spans="1:42" s="189" customFormat="1" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:42" s="189" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B7" s="193"/>
       <c r="C7" s="194"/>
       <c r="D7" s="194"/>
@@ -39585,7 +39591,7 @@
       <c r="O7" s="194"/>
       <c r="Z7" s="202"/>
     </row>
-    <row r="8" spans="1:42" s="189" customFormat="1" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:42" s="189" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B8" s="190" t="s">
         <v>66</v>
       </c>
@@ -39602,7 +39608,7 @@
       <c r="O8" s="194"/>
       <c r="Z8" s="202"/>
     </row>
-    <row r="9" spans="1:42" s="189" customFormat="1" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:42" s="189" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B9" s="192" t="s">
         <v>58</v>
       </c>
@@ -39629,7 +39635,7 @@
       <c r="O9" s="194"/>
       <c r="Z9" s="202"/>
     </row>
-    <row r="10" spans="1:42" s="189" customFormat="1" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:42" s="189" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B10" s="192" t="s">
         <v>64</v>
       </c>
@@ -39656,7 +39662,7 @@
       <c r="O10" s="194"/>
       <c r="Z10" s="202"/>
     </row>
-    <row r="11" spans="1:42" s="189" customFormat="1" ht="16" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="11" spans="1:42" s="189" customFormat="1" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B11" s="193"/>
       <c r="C11" s="194"/>
       <c r="D11" s="194"/>
@@ -39665,7 +39671,7 @@
       <c r="G11" s="194"/>
       <c r="Z11" s="202"/>
     </row>
-    <row r="12" spans="1:42" ht="24" thickBot="1" x14ac:dyDescent="0.6">
+    <row r="12" spans="1:42" ht="24" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A12" s="90"/>
       <c r="B12" s="25" t="s">
         <v>50</v>
@@ -39721,7 +39727,7 @@
       <c r="AO12" s="175"/>
       <c r="AP12" s="176"/>
     </row>
-    <row r="13" spans="1:42" ht="16" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="13" spans="1:42" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A13" s="91"/>
       <c r="B13" s="40"/>
       <c r="C13" s="92" t="s">
@@ -39789,7 +39795,7 @@
       <c r="AO13" s="153"/>
       <c r="AP13" s="155"/>
     </row>
-    <row r="14" spans="1:42" s="1" customFormat="1" ht="21.5" thickBot="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="14" spans="1:42" s="1" customFormat="1" ht="21.75" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A14" s="94" t="s">
         <v>0</v>
       </c>
@@ -39907,7 +39913,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="15" spans="1:42" s="1" customFormat="1" ht="18.5" x14ac:dyDescent="0.45">
+    <row r="15" spans="1:42" s="1" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A15" s="4"/>
       <c r="B15" s="18" t="s">
         <v>95</v>
@@ -39956,7 +39962,7 @@
       <c r="AO15" s="5"/>
       <c r="AP15" s="9"/>
     </row>
-    <row r="16" spans="1:42" ht="18.5" x14ac:dyDescent="0.45">
+    <row r="16" spans="1:42" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A16" s="95"/>
       <c r="B16" s="19"/>
       <c r="C16" s="11"/>
@@ -40096,7 +40102,7 @@
         <v/>
       </c>
     </row>
-    <row r="17" spans="1:42" ht="18.5" x14ac:dyDescent="0.45">
+    <row r="17" spans="1:42" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A17" s="96"/>
       <c r="B17" s="146" t="s">
         <v>65</v>
@@ -40145,7 +40151,7 @@
       <c r="AO17" s="73"/>
       <c r="AP17" s="71"/>
     </row>
-    <row r="18" spans="1:42" ht="18.5" x14ac:dyDescent="0.45">
+    <row r="18" spans="1:42" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A18" s="95"/>
       <c r="B18" s="19" t="s">
         <v>7</v>
@@ -40293,7 +40299,7 @@
         <v>13.219206000000002</v>
       </c>
     </row>
-    <row r="19" spans="1:42" ht="18.5" x14ac:dyDescent="0.45">
+    <row r="19" spans="1:42" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A19" s="95"/>
       <c r="B19" s="19" t="s">
         <v>11</v>
@@ -40441,7 +40447,7 @@
         <v>14.426997000000002</v>
       </c>
     </row>
-    <row r="20" spans="1:42" ht="18.5" x14ac:dyDescent="0.45">
+    <row r="20" spans="1:42" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A20" s="95"/>
       <c r="B20" s="19" t="s">
         <v>12</v>
@@ -40589,7 +40595,7 @@
         <v>21.278400000000001</v>
       </c>
     </row>
-    <row r="21" spans="1:42" ht="18.5" x14ac:dyDescent="0.45">
+    <row r="21" spans="1:42" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A21" s="95"/>
       <c r="B21" s="19" t="s">
         <v>13</v>
@@ -40737,7 +40743,7 @@
         <v>9.5631900000000005</v>
       </c>
     </row>
-    <row r="22" spans="1:42" ht="18.5" x14ac:dyDescent="0.45">
+    <row r="22" spans="1:42" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A22" s="95"/>
       <c r="B22" s="19" t="s">
         <v>14</v>
@@ -40885,7 +40891,7 @@
         <v>8.5621380000000027</v>
       </c>
     </row>
-    <row r="23" spans="1:42" ht="18.5" x14ac:dyDescent="0.45">
+    <row r="23" spans="1:42" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A23" s="95"/>
       <c r="B23" s="19" t="s">
         <v>8</v>
@@ -41033,7 +41039,7 @@
         <v>15.032705999999999</v>
       </c>
     </row>
-    <row r="24" spans="1:42" ht="18.5" x14ac:dyDescent="0.45">
+    <row r="24" spans="1:42" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A24" s="95"/>
       <c r="B24" s="19" t="s">
         <v>9</v>
@@ -41181,7 +41187,7 @@
         <v>12.145614</v>
       </c>
     </row>
-    <row r="25" spans="1:42" ht="18.5" x14ac:dyDescent="0.45">
+    <row r="25" spans="1:42" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A25" s="95"/>
       <c r="B25" s="19" t="s">
         <v>19</v>
@@ -41329,7 +41335,7 @@
         <v>25.757745000000003</v>
       </c>
     </row>
-    <row r="26" spans="1:42" ht="18.5" x14ac:dyDescent="0.45">
+    <row r="26" spans="1:42" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A26" s="95"/>
       <c r="B26" s="19" t="s">
         <v>15</v>
@@ -41477,7 +41483,7 @@
         <v>18.775770000000001</v>
       </c>
     </row>
-    <row r="27" spans="1:42" ht="18.5" x14ac:dyDescent="0.45">
+    <row r="27" spans="1:42" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A27" s="95"/>
       <c r="B27" s="19"/>
       <c r="C27" s="11"/>
@@ -41521,7 +41527,7 @@
       <c r="AO27" s="44"/>
       <c r="AP27" s="42"/>
     </row>
-    <row r="28" spans="1:42" ht="18.5" x14ac:dyDescent="0.45">
+    <row r="28" spans="1:42" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A28" s="95"/>
       <c r="B28" s="19"/>
       <c r="C28" s="11"/>
@@ -41565,7 +41571,7 @@
       <c r="AO28" s="44"/>
       <c r="AP28" s="42"/>
     </row>
-    <row r="29" spans="1:42" ht="18.5" x14ac:dyDescent="0.45">
+    <row r="29" spans="1:42" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A29" s="95"/>
       <c r="B29" s="19"/>
       <c r="C29" s="11"/>
@@ -41705,7 +41711,7 @@
         <v/>
       </c>
     </row>
-    <row r="30" spans="1:42" ht="18.5" x14ac:dyDescent="0.45">
+    <row r="30" spans="1:42" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A30" s="95"/>
       <c r="B30" s="19"/>
       <c r="C30" s="11"/>
@@ -41749,7 +41755,7 @@
       <c r="AO30" s="44"/>
       <c r="AP30" s="42"/>
     </row>
-    <row r="31" spans="1:42" ht="18.5" x14ac:dyDescent="0.45">
+    <row r="31" spans="1:42" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A31" s="95"/>
       <c r="B31" s="269" t="s">
         <v>129</v>
@@ -41897,7 +41903,7 @@
         <v>6.0360960000000023</v>
       </c>
     </row>
-    <row r="32" spans="1:42" ht="18.5" x14ac:dyDescent="0.45">
+    <row r="32" spans="1:42" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A32" s="95"/>
       <c r="B32" s="269" t="s">
         <v>128</v>
@@ -42045,7 +42051,7 @@
         <v>6.4004160000000008</v>
       </c>
     </row>
-    <row r="33" spans="1:42" ht="18.5" x14ac:dyDescent="0.45">
+    <row r="33" spans="1:42" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A33" s="95"/>
       <c r="B33" s="269" t="s">
         <v>125</v>
@@ -42193,7 +42199,7 @@
         <v>7.38408</v>
       </c>
     </row>
-    <row r="34" spans="1:42" ht="18.5" x14ac:dyDescent="0.45">
+    <row r="34" spans="1:42" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A34" s="95"/>
       <c r="B34" s="269" t="s">
         <v>126</v>
@@ -42341,7 +42347,7 @@
         <v>11.755920000000001</v>
       </c>
     </row>
-    <row r="35" spans="1:42" ht="18.5" x14ac:dyDescent="0.45">
+    <row r="35" spans="1:42" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A35" s="95"/>
       <c r="B35" s="269" t="s">
         <v>127</v>
@@ -42489,7 +42495,7 @@
         <v>8.3313120000000023</v>
       </c>
     </row>
-    <row r="36" spans="1:42" ht="18.5" x14ac:dyDescent="0.45">
+    <row r="36" spans="1:42" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A36" s="95"/>
       <c r="B36" s="269" t="s">
         <v>131</v>
@@ -42637,7 +42643,7 @@
         <v>8.1127200000000013</v>
       </c>
     </row>
-    <row r="37" spans="1:42" ht="18.5" x14ac:dyDescent="0.45">
+    <row r="37" spans="1:42" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A37" s="95"/>
       <c r="B37" s="19"/>
       <c r="C37" s="11"/>
@@ -42774,7 +42780,7 @@
         <v/>
       </c>
     </row>
-    <row r="38" spans="1:42" ht="18.5" x14ac:dyDescent="0.45">
+    <row r="38" spans="1:42" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A38" s="95"/>
       <c r="B38" s="19"/>
       <c r="C38" s="11"/>
@@ -42911,7 +42917,7 @@
         <v/>
       </c>
     </row>
-    <row r="39" spans="1:42" ht="18.5" x14ac:dyDescent="0.45">
+    <row r="39" spans="1:42" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A39" s="95"/>
       <c r="B39" s="19"/>
       <c r="C39" s="11"/>
@@ -43051,7 +43057,7 @@
         <v/>
       </c>
     </row>
-    <row r="40" spans="1:42" ht="18.5" x14ac:dyDescent="0.45">
+    <row r="40" spans="1:42" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A40" s="97"/>
       <c r="B40" s="147" t="s">
         <v>10</v>
@@ -43109,7 +43115,7 @@
       <c r="AO40" s="86"/>
       <c r="AP40" s="84"/>
     </row>
-    <row r="41" spans="1:42" ht="18.5" x14ac:dyDescent="0.45">
+    <row r="41" spans="1:42" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A41" s="95"/>
       <c r="B41" s="19" t="s">
         <v>16</v>
@@ -43257,7 +43263,7 @@
         <v>37.078200000000002</v>
       </c>
     </row>
-    <row r="42" spans="1:42" ht="18.5" x14ac:dyDescent="0.45">
+    <row r="42" spans="1:42" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A42" s="95"/>
       <c r="B42" s="19" t="s">
         <v>17</v>
@@ -43405,7 +43411,7 @@
         <v>15.866999999999999</v>
       </c>
     </row>
-    <row r="43" spans="1:42" ht="18.5" x14ac:dyDescent="0.45">
+    <row r="43" spans="1:42" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A43" s="95"/>
       <c r="B43" s="19" t="s">
         <v>18</v>
@@ -43553,7 +43559,7 @@
         <v>45.070200000000007</v>
       </c>
     </row>
-    <row r="44" spans="1:42" ht="18.5" x14ac:dyDescent="0.45">
+    <row r="44" spans="1:42" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A44" s="95"/>
       <c r="B44" s="19"/>
       <c r="C44" s="11"/>
@@ -43693,7 +43699,7 @@
         <v/>
       </c>
     </row>
-    <row r="45" spans="1:42" ht="18.5" x14ac:dyDescent="0.45">
+    <row r="45" spans="1:42" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A45" s="95"/>
       <c r="B45" s="19"/>
       <c r="C45" s="11"/>
@@ -43833,7 +43839,7 @@
         <v/>
       </c>
     </row>
-    <row r="46" spans="1:42" ht="18.5" x14ac:dyDescent="0.45">
+    <row r="46" spans="1:42" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A46" s="95"/>
       <c r="B46" s="19"/>
       <c r="C46" s="11"/>
@@ -43973,7 +43979,7 @@
         <v/>
       </c>
     </row>
-    <row r="47" spans="1:42" ht="18.5" x14ac:dyDescent="0.45">
+    <row r="47" spans="1:42" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A47" s="95"/>
       <c r="B47" s="19"/>
       <c r="C47" s="11"/>
@@ -44113,7 +44119,7 @@
         <v/>
       </c>
     </row>
-    <row r="48" spans="1:42" ht="18.5" x14ac:dyDescent="0.45">
+    <row r="48" spans="1:42" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A48" s="98"/>
       <c r="B48" s="3" t="s">
         <v>20</v>
@@ -44171,7 +44177,7 @@
       <c r="AO48" s="61"/>
       <c r="AP48" s="204"/>
     </row>
-    <row r="49" spans="1:42" ht="18.5" x14ac:dyDescent="0.45">
+    <row r="49" spans="1:42" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A49" s="95"/>
       <c r="B49" s="19" t="s">
         <v>21</v>
@@ -44319,7 +44325,7 @@
         <v>12.3</v>
       </c>
     </row>
-    <row r="50" spans="1:42" ht="18.5" x14ac:dyDescent="0.45">
+    <row r="50" spans="1:42" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A50" s="95"/>
       <c r="B50" s="19" t="s">
         <v>22</v>
@@ -44463,7 +44469,7 @@
         <v/>
       </c>
     </row>
-    <row r="51" spans="1:42" ht="18.5" x14ac:dyDescent="0.45">
+    <row r="51" spans="1:42" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A51" s="95"/>
       <c r="B51" s="19"/>
       <c r="C51" s="11"/>
@@ -44603,7 +44609,7 @@
         <v/>
       </c>
     </row>
-    <row r="52" spans="1:42" ht="18.5" x14ac:dyDescent="0.45">
+    <row r="52" spans="1:42" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A52" s="95"/>
       <c r="B52" s="19" t="s">
         <v>23</v>
@@ -44751,7 +44757,7 @@
         <v>13.020000000000001</v>
       </c>
     </row>
-    <row r="53" spans="1:42" ht="19" thickBot="1" x14ac:dyDescent="0.5">
+    <row r="53" spans="1:42" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A53" s="99"/>
       <c r="B53" s="100"/>
       <c r="C53" s="13"/>
@@ -44888,23 +44894,23 @@
         <v/>
       </c>
     </row>
-    <row r="61" spans="1:42" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="61" spans="1:42" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B61" s="269"/>
       <c r="C61" s="259"/>
     </row>
-    <row r="62" spans="1:42" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="62" spans="1:42" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B62" s="269"/>
       <c r="C62" s="259"/>
     </row>
-    <row r="63" spans="1:42" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="63" spans="1:42" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B63" s="269"/>
       <c r="C63" s="259"/>
     </row>
-    <row r="64" spans="1:42" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="64" spans="1:42" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B64" s="269"/>
       <c r="C64" s="259"/>
     </row>
-    <row r="65" spans="2:3" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="65" spans="2:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B65" s="269"/>
       <c r="C65" s="259"/>
     </row>
@@ -44923,58 +44929,58 @@
       <selection activeCell="B21" sqref="B21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="4" customWidth="1"/>
     <col min="2" max="2" width="58" customWidth="1"/>
-    <col min="3" max="3" width="16.453125" customWidth="1"/>
+    <col min="3" max="3" width="16.42578125" customWidth="1"/>
     <col min="4" max="4" width="15" customWidth="1"/>
-    <col min="5" max="5" width="12.08984375" customWidth="1"/>
-    <col min="6" max="6" width="17.453125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="9.90625" customWidth="1"/>
-    <col min="8" max="8" width="13.36328125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="12.140625" customWidth="1"/>
+    <col min="6" max="6" width="17.42578125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="9.85546875" customWidth="1"/>
+    <col min="8" max="8" width="13.42578125" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="5" customWidth="1"/>
-    <col min="10" max="10" width="16.36328125" customWidth="1"/>
-    <col min="11" max="11" width="15.6328125" customWidth="1"/>
-    <col min="12" max="12" width="8.453125" customWidth="1"/>
-    <col min="13" max="13" width="19.453125" customWidth="1"/>
-    <col min="14" max="14" width="8.08984375" customWidth="1"/>
-    <col min="15" max="15" width="9.453125" customWidth="1"/>
-    <col min="16" max="16" width="6.90625" customWidth="1"/>
+    <col min="10" max="10" width="16.42578125" customWidth="1"/>
+    <col min="11" max="11" width="15.5703125" customWidth="1"/>
+    <col min="12" max="12" width="8.42578125" customWidth="1"/>
+    <col min="13" max="13" width="19.42578125" customWidth="1"/>
+    <col min="14" max="14" width="8.140625" customWidth="1"/>
+    <col min="15" max="15" width="9.42578125" customWidth="1"/>
+    <col min="16" max="16" width="6.85546875" customWidth="1"/>
     <col min="17" max="17" width="5" customWidth="1"/>
-    <col min="18" max="18" width="15.54296875" customWidth="1"/>
-    <col min="19" max="19" width="12.36328125" customWidth="1"/>
-    <col min="20" max="20" width="8.6328125" customWidth="1"/>
-    <col min="21" max="21" width="23.6328125" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="7.6328125" customWidth="1"/>
-    <col min="23" max="24" width="8.90625" customWidth="1"/>
-    <col min="25" max="25" width="5.6328125" customWidth="1"/>
-    <col min="26" max="26" width="41.6328125" style="200" customWidth="1"/>
-    <col min="27" max="27" width="5.6328125" customWidth="1"/>
-    <col min="28" max="28" width="15.6328125" customWidth="1"/>
-    <col min="29" max="29" width="12.54296875" customWidth="1"/>
+    <col min="18" max="18" width="15.5703125" customWidth="1"/>
+    <col min="19" max="19" width="12.42578125" customWidth="1"/>
+    <col min="20" max="20" width="8.5703125" customWidth="1"/>
+    <col min="21" max="21" width="23.5703125" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="7.5703125" customWidth="1"/>
+    <col min="23" max="24" width="8.85546875" customWidth="1"/>
+    <col min="25" max="25" width="5.5703125" customWidth="1"/>
+    <col min="26" max="26" width="41.5703125" style="200" customWidth="1"/>
+    <col min="27" max="27" width="5.5703125" customWidth="1"/>
+    <col min="28" max="28" width="15.5703125" customWidth="1"/>
+    <col min="29" max="29" width="12.5703125" customWidth="1"/>
     <col min="30" max="30" width="9" customWidth="1"/>
-    <col min="31" max="31" width="18.6328125" customWidth="1"/>
-    <col min="32" max="32" width="9.453125" customWidth="1"/>
-    <col min="33" max="33" width="10.453125" customWidth="1"/>
-    <col min="34" max="34" width="7.6328125" customWidth="1"/>
-    <col min="35" max="35" width="5.36328125" customWidth="1"/>
+    <col min="31" max="31" width="18.5703125" customWidth="1"/>
+    <col min="32" max="32" width="9.42578125" customWidth="1"/>
+    <col min="33" max="33" width="10.42578125" customWidth="1"/>
+    <col min="34" max="34" width="7.5703125" customWidth="1"/>
+    <col min="35" max="35" width="5.42578125" customWidth="1"/>
     <col min="36" max="36" width="13" customWidth="1"/>
-    <col min="37" max="37" width="11.90625" customWidth="1"/>
-    <col min="38" max="38" width="9.6328125" customWidth="1"/>
-    <col min="39" max="39" width="19.08984375" customWidth="1"/>
-    <col min="40" max="40" width="8.08984375" customWidth="1"/>
-    <col min="41" max="42" width="8.54296875" customWidth="1"/>
+    <col min="37" max="37" width="11.85546875" customWidth="1"/>
+    <col min="38" max="38" width="9.5703125" customWidth="1"/>
+    <col min="39" max="39" width="19.140625" customWidth="1"/>
+    <col min="40" max="40" width="8.140625" customWidth="1"/>
+    <col min="41" max="42" width="8.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:42" ht="103.5" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="2" spans="1:42" s="108" customFormat="1" ht="46" x14ac:dyDescent="1">
+    <row r="1" spans="1:42" ht="103.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="2" spans="1:42" s="108" customFormat="1" ht="46.5" x14ac:dyDescent="0.7">
       <c r="B2" s="108" t="s">
         <v>56</v>
       </c>
       <c r="Z2" s="201"/>
     </row>
-    <row r="3" spans="1:42" s="108" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="1">
+    <row r="3" spans="1:42" s="108" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.7">
       <c r="A3" s="189"/>
       <c r="B3" s="189"/>
       <c r="C3" s="189"/>
@@ -45018,7 +45024,7 @@
       <c r="AO3" s="189"/>
       <c r="AP3" s="189"/>
     </row>
-    <row r="4" spans="1:42" s="189" customFormat="1" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:42" s="189" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B4" s="190" t="s">
         <v>57</v>
       </c>
@@ -45035,7 +45041,7 @@
       <c r="O4" s="195"/>
       <c r="Z4" s="202"/>
     </row>
-    <row r="5" spans="1:42" s="189" customFormat="1" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:42" s="189" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B5" s="192" t="s">
         <v>58</v>
       </c>
@@ -45062,7 +45068,7 @@
       <c r="O5" s="197"/>
       <c r="Z5" s="202"/>
     </row>
-    <row r="6" spans="1:42" s="189" customFormat="1" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:42" s="189" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B6" s="192" t="s">
         <v>59</v>
       </c>
@@ -45089,7 +45095,7 @@
       <c r="O6" s="197"/>
       <c r="Z6" s="202"/>
     </row>
-    <row r="7" spans="1:42" s="189" customFormat="1" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:42" s="189" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B7" s="193"/>
       <c r="C7" s="194"/>
       <c r="D7" s="194"/>
@@ -45104,7 +45110,7 @@
       <c r="O7" s="194"/>
       <c r="Z7" s="202"/>
     </row>
-    <row r="8" spans="1:42" s="189" customFormat="1" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:42" s="189" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B8" s="190" t="s">
         <v>66</v>
       </c>
@@ -45121,7 +45127,7 @@
       <c r="O8" s="194"/>
       <c r="Z8" s="202"/>
     </row>
-    <row r="9" spans="1:42" s="189" customFormat="1" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:42" s="189" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B9" s="192" t="s">
         <v>58</v>
       </c>
@@ -45148,7 +45154,7 @@
       <c r="O9" s="194"/>
       <c r="Z9" s="202"/>
     </row>
-    <row r="10" spans="1:42" s="189" customFormat="1" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:42" s="189" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B10" s="192" t="s">
         <v>64</v>
       </c>
@@ -45175,7 +45181,7 @@
       <c r="O10" s="194"/>
       <c r="Z10" s="202"/>
     </row>
-    <row r="11" spans="1:42" s="189" customFormat="1" ht="16" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="11" spans="1:42" s="189" customFormat="1" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B11" s="193"/>
       <c r="C11" s="194"/>
       <c r="D11" s="194"/>
@@ -45184,7 +45190,7 @@
       <c r="G11" s="194"/>
       <c r="Z11" s="202"/>
     </row>
-    <row r="12" spans="1:42" ht="24" thickBot="1" x14ac:dyDescent="0.6">
+    <row r="12" spans="1:42" ht="24" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A12" s="90"/>
       <c r="B12" s="25" t="s">
         <v>50</v>
@@ -45240,7 +45246,7 @@
       <c r="AO12" s="175"/>
       <c r="AP12" s="176"/>
     </row>
-    <row r="13" spans="1:42" ht="16" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="13" spans="1:42" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A13" s="91"/>
       <c r="B13" s="40"/>
       <c r="C13" s="92" t="s">
@@ -45308,7 +45314,7 @@
       <c r="AO13" s="153"/>
       <c r="AP13" s="155"/>
     </row>
-    <row r="14" spans="1:42" s="1" customFormat="1" ht="21.5" thickBot="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="14" spans="1:42" s="1" customFormat="1" ht="21.75" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A14" s="94" t="s">
         <v>0</v>
       </c>
@@ -45426,7 +45432,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="15" spans="1:42" s="1" customFormat="1" ht="18.5" x14ac:dyDescent="0.45">
+    <row r="15" spans="1:42" s="1" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A15" s="4"/>
       <c r="B15" s="18" t="s">
         <v>96</v>
@@ -45475,7 +45481,7 @@
       <c r="AO15" s="5"/>
       <c r="AP15" s="9"/>
     </row>
-    <row r="16" spans="1:42" ht="18.5" x14ac:dyDescent="0.45">
+    <row r="16" spans="1:42" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A16" s="95"/>
       <c r="B16" s="246" t="s">
         <v>5</v>
@@ -45623,7 +45629,7 @@
         <v>4.6845600000000012</v>
       </c>
     </row>
-    <row r="17" spans="1:42" ht="18.5" x14ac:dyDescent="0.45">
+    <row r="17" spans="1:42" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A17" s="95"/>
       <c r="B17" s="19"/>
       <c r="C17" s="11"/>
@@ -45763,7 +45769,7 @@
         <v/>
       </c>
     </row>
-    <row r="18" spans="1:42" ht="18.5" x14ac:dyDescent="0.45">
+    <row r="18" spans="1:42" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A18" s="96"/>
       <c r="B18" s="146" t="s">
         <v>65</v>
@@ -45812,7 +45818,7 @@
       <c r="AO18" s="73"/>
       <c r="AP18" s="71"/>
     </row>
-    <row r="19" spans="1:42" ht="18.5" x14ac:dyDescent="0.45">
+    <row r="19" spans="1:42" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A19" s="95"/>
       <c r="B19" s="19" t="s">
         <v>97</v>
@@ -45960,7 +45966,7 @@
         <v>8.9901000000000018</v>
       </c>
     </row>
-    <row r="20" spans="1:42" ht="18.5" x14ac:dyDescent="0.45">
+    <row r="20" spans="1:42" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A20" s="95"/>
       <c r="B20" s="19" t="s">
         <v>98</v>
@@ -46108,7 +46114,7 @@
         <v>7.6860000000000017</v>
       </c>
     </row>
-    <row r="21" spans="1:42" ht="18.5" x14ac:dyDescent="0.45">
+    <row r="21" spans="1:42" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A21" s="95"/>
       <c r="B21" s="19" t="s">
         <v>99</v>
@@ -46256,7 +46262,7 @@
         <v>7.4970000000000008</v>
       </c>
     </row>
-    <row r="22" spans="1:42" ht="18.5" x14ac:dyDescent="0.45">
+    <row r="22" spans="1:42" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A22" s="95"/>
       <c r="B22" s="19" t="s">
         <v>100</v>
@@ -46404,7 +46410,7 @@
         <v>7.742700000000001</v>
       </c>
     </row>
-    <row r="23" spans="1:42" ht="18.5" x14ac:dyDescent="0.45">
+    <row r="23" spans="1:42" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A23" s="95"/>
       <c r="B23" s="19" t="s">
         <v>101</v>
@@ -46552,7 +46558,7 @@
         <v>6.9839999999999991</v>
       </c>
     </row>
-    <row r="24" spans="1:42" ht="18.5" x14ac:dyDescent="0.45">
+    <row r="24" spans="1:42" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A24" s="95"/>
       <c r="B24" s="19" t="s">
         <v>102</v>
@@ -46700,7 +46706,7 @@
         <v>7.9586999999999986</v>
       </c>
     </row>
-    <row r="25" spans="1:42" ht="18.5" x14ac:dyDescent="0.45">
+    <row r="25" spans="1:42" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A25" s="95"/>
       <c r="B25" s="19" t="s">
         <v>103</v>
@@ -46848,7 +46854,7 @@
         <v>7.3890000000000002</v>
       </c>
     </row>
-    <row r="26" spans="1:42" ht="18.5" x14ac:dyDescent="0.45">
+    <row r="26" spans="1:42" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A26" s="95"/>
       <c r="B26" s="19" t="s">
         <v>104</v>
@@ -46996,7 +47002,7 @@
         <v>6.1443000000000003</v>
       </c>
     </row>
-    <row r="27" spans="1:42" ht="18.5" x14ac:dyDescent="0.45">
+    <row r="27" spans="1:42" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A27" s="95"/>
       <c r="B27" s="19" t="s">
         <v>124</v>
@@ -47144,7 +47150,7 @@
         <v>7.1730000000000009</v>
       </c>
     </row>
-    <row r="28" spans="1:42" ht="18.5" x14ac:dyDescent="0.45">
+    <row r="28" spans="1:42" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A28" s="95"/>
       <c r="B28" s="19" t="s">
         <v>105</v>
@@ -47292,7 +47298,7 @@
         <v>6.8301000000000007</v>
       </c>
     </row>
-    <row r="29" spans="1:42" ht="18.5" x14ac:dyDescent="0.45">
+    <row r="29" spans="1:42" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A29" s="95"/>
       <c r="B29" s="19" t="s">
         <v>106</v>
@@ -47440,7 +47446,7 @@
         <v>6.8301000000000007</v>
       </c>
     </row>
-    <row r="30" spans="1:42" ht="18.5" x14ac:dyDescent="0.45">
+    <row r="30" spans="1:42" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A30" s="95"/>
       <c r="B30" s="19" t="s">
         <v>112</v>
@@ -47586,7 +47592,7 @@
         <v>0.31500000000000006</v>
       </c>
     </row>
-    <row r="31" spans="1:42" ht="18.5" x14ac:dyDescent="0.45">
+    <row r="31" spans="1:42" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A31" s="95"/>
       <c r="B31" s="19" t="s">
         <v>113</v>
@@ -47732,7 +47738,7 @@
         <v>0.31500000000000006</v>
       </c>
     </row>
-    <row r="32" spans="1:42" ht="18.5" x14ac:dyDescent="0.45">
+    <row r="32" spans="1:42" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A32" s="95"/>
       <c r="B32" s="19" t="s">
         <v>114</v>
@@ -47878,7 +47884,7 @@
         <v>0.31500000000000006</v>
       </c>
     </row>
-    <row r="33" spans="1:42" ht="18.5" x14ac:dyDescent="0.45">
+    <row r="33" spans="1:42" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A33" s="95"/>
       <c r="B33" s="19" t="s">
         <v>115</v>
@@ -48024,7 +48030,7 @@
         <v>0.31500000000000006</v>
       </c>
     </row>
-    <row r="34" spans="1:42" ht="18.5" x14ac:dyDescent="0.45">
+    <row r="34" spans="1:42" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A34" s="95"/>
       <c r="B34" s="19" t="s">
         <v>116</v>
@@ -48170,7 +48176,7 @@
         <v>0.31500000000000006</v>
       </c>
     </row>
-    <row r="35" spans="1:42" ht="18.5" x14ac:dyDescent="0.45">
+    <row r="35" spans="1:42" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A35" s="95"/>
       <c r="B35" s="19" t="s">
         <v>117</v>
@@ -48316,7 +48322,7 @@
         <v>0.31500000000000006</v>
       </c>
     </row>
-    <row r="36" spans="1:42" ht="18.5" x14ac:dyDescent="0.45">
+    <row r="36" spans="1:42" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A36" s="95"/>
       <c r="B36" s="19"/>
       <c r="C36" s="11"/>
@@ -48456,7 +48462,7 @@
         <v/>
       </c>
     </row>
-    <row r="37" spans="1:42" ht="18.5" x14ac:dyDescent="0.45">
+    <row r="37" spans="1:42" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A37" s="95"/>
       <c r="B37" s="19"/>
       <c r="C37" s="11"/>
@@ -48596,7 +48602,7 @@
         <v/>
       </c>
     </row>
-    <row r="38" spans="1:42" ht="18.5" x14ac:dyDescent="0.45">
+    <row r="38" spans="1:42" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A38" s="95"/>
       <c r="B38" s="19"/>
       <c r="C38" s="11"/>
@@ -48736,7 +48742,7 @@
         <v/>
       </c>
     </row>
-    <row r="39" spans="1:42" ht="18.5" x14ac:dyDescent="0.45">
+    <row r="39" spans="1:42" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A39" s="95"/>
       <c r="B39" s="19"/>
       <c r="C39" s="11"/>
@@ -48876,7 +48882,7 @@
         <v/>
       </c>
     </row>
-    <row r="40" spans="1:42" ht="18.5" x14ac:dyDescent="0.45">
+    <row r="40" spans="1:42" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A40" s="95"/>
       <c r="B40" s="19"/>
       <c r="C40" s="11"/>
@@ -49016,7 +49022,7 @@
         <v/>
       </c>
     </row>
-    <row r="41" spans="1:42" ht="18.5" x14ac:dyDescent="0.45">
+    <row r="41" spans="1:42" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A41" s="95"/>
       <c r="B41" s="19"/>
       <c r="C41" s="11"/>
@@ -49156,7 +49162,7 @@
         <v/>
       </c>
     </row>
-    <row r="42" spans="1:42" ht="18.5" x14ac:dyDescent="0.45">
+    <row r="42" spans="1:42" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A42" s="98"/>
       <c r="B42" s="3" t="s">
         <v>20</v>
@@ -49214,7 +49220,7 @@
       <c r="AO42" s="61"/>
       <c r="AP42" s="204"/>
     </row>
-    <row r="43" spans="1:42" ht="18.5" x14ac:dyDescent="0.45">
+    <row r="43" spans="1:42" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A43" s="95"/>
       <c r="B43" s="19" t="s">
         <v>21</v>
@@ -49362,7 +49368,7 @@
         <v>12.3</v>
       </c>
     </row>
-    <row r="44" spans="1:42" ht="18.5" x14ac:dyDescent="0.45">
+    <row r="44" spans="1:42" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A44" s="95"/>
       <c r="B44" s="19" t="s">
         <v>22</v>
@@ -49506,7 +49512,7 @@
         <v/>
       </c>
     </row>
-    <row r="45" spans="1:42" ht="18.5" x14ac:dyDescent="0.45">
+    <row r="45" spans="1:42" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A45" s="95"/>
       <c r="B45" s="19"/>
       <c r="C45" s="11"/>
@@ -49646,7 +49652,7 @@
         <v/>
       </c>
     </row>
-    <row r="46" spans="1:42" ht="18.5" x14ac:dyDescent="0.45">
+    <row r="46" spans="1:42" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A46" s="95"/>
       <c r="B46" s="19" t="s">
         <v>23</v>
@@ -49794,7 +49800,7 @@
         <v>13.020000000000001</v>
       </c>
     </row>
-    <row r="47" spans="1:42" ht="19" thickBot="1" x14ac:dyDescent="0.5">
+    <row r="47" spans="1:42" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A47" s="99"/>
       <c r="B47" s="100"/>
       <c r="C47" s="13"/>

</xml_diff>